<commit_message>
287, 300 reruns for fast run
</commit_message>
<xml_diff>
--- a/fast run results.xlsx
+++ b/fast run results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CE_yto16\Documents\Uni stuff\Year 4\Research Project\gaussian-process-rto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - Imperial College London\School Work\Year 4\Research project\GITTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0EED937-D1BA-42D9-9FEE-5D74DA713A81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{5B84B35A-4784-4095-8A35-73569DC69E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,7 +492,7 @@
   <dimension ref="A1:AA443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="W257" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C392" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="AA264" sqref="AA264"/>
@@ -35103,15 +35103,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F19637432BAAAA4E8B613AD4CF549CCD" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1a882fa068e99a90637f35d72ee4199">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f35accf0-cd8f-4670-ac72-d44f2085032d" xmlns:ns4="95507c7c-a837-40bb-8a3d-470d6a1609d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9631af341c2920228165fa301a4a4d8" ns3:_="" ns4:_="">
     <xsd:import namespace="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
@@ -35320,6 +35311,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A6ED6D0-FE53-4BFC-8DEF-82D0D9F0E993}">
   <ds:schemaRefs>
@@ -35338,14 +35338,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2B5FC1-AD94-452E-B48E-8A2F9B1C8C34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0B59684-2680-485A-B9CC-B3EE2FE02703}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35362,4 +35354,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2B5FC1-AD94-452E-B48E-8A2F9B1C8C34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated fast run reruns results
</commit_message>
<xml_diff>
--- a/fast run results.xlsx
+++ b/fast run results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - Imperial College London\School Work\Year 4\Research project\GITTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{5B84B35A-4784-4095-8A35-73569DC69E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="114_{5B84B35A-4784-4095-8A35-73569DC69E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0B3559A-7F38-4F5D-B096-DE29307C09B3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="32">
   <si>
     <t>Inputs - Sour gas flowrate</t>
   </si>
@@ -143,7 +143,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,12 +175,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +500,10 @@
   <dimension ref="A1:AA443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C392" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Q411" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA264" sqref="AA264"/>
+      <selection pane="bottomRight" activeCell="S417" sqref="S417"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32218,11 +32226,86 @@
       </c>
     </row>
     <row r="405" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A405" s="2">
+      <c r="A405" s="3">
         <v>287</v>
       </c>
-      <c r="B405" s="2">
+      <c r="B405">
         <v>98000</v>
+      </c>
+      <c r="C405">
+        <v>861</v>
+      </c>
+      <c r="D405">
+        <v>98000</v>
+      </c>
+      <c r="E405">
+        <v>0.1</v>
+      </c>
+      <c r="F405">
+        <v>287</v>
+      </c>
+      <c r="G405">
+        <v>6.3122999999999999E-2</v>
+      </c>
+      <c r="H405">
+        <v>180</v>
+      </c>
+      <c r="I405">
+        <v>180</v>
+      </c>
+      <c r="J405">
+        <v>170</v>
+      </c>
+      <c r="K405">
+        <v>170</v>
+      </c>
+      <c r="L405">
+        <v>40</v>
+      </c>
+      <c r="M405">
+        <v>35.005428999999999</v>
+      </c>
+      <c r="N405">
+        <v>89.799657999999994</v>
+      </c>
+      <c r="O405">
+        <v>25</v>
+      </c>
+      <c r="P405">
+        <v>3.6606E-2</v>
+      </c>
+      <c r="Q405">
+        <v>0.144509</v>
+      </c>
+      <c r="R405">
+        <v>0.81888499999999997</v>
+      </c>
+      <c r="S405">
+        <v>-10460.583111</v>
+      </c>
+      <c r="T405">
+        <v>176872.45305400001</v>
+      </c>
+      <c r="U405">
+        <v>67354.372323000003</v>
+      </c>
+      <c r="V405">
+        <v>33.497601000000003</v>
+      </c>
+      <c r="W405">
+        <v>49.870942999999997</v>
+      </c>
+      <c r="X405">
+        <v>26.904333000000001</v>
+      </c>
+      <c r="Y405">
+        <v>15.665694999999999</v>
+      </c>
+      <c r="Z405">
+        <v>33.156154999999998</v>
+      </c>
+      <c r="AA405">
+        <v>-9.7243999999999997E-2</v>
       </c>
     </row>
     <row r="406" spans="1:27" x14ac:dyDescent="0.35">
@@ -32230,13 +32313,13 @@
         <v>287</v>
       </c>
       <c r="B406">
-        <v>100000</v>
+        <v>104000</v>
       </c>
       <c r="C406">
         <v>861</v>
       </c>
       <c r="D406">
-        <v>100000</v>
+        <v>104000</v>
       </c>
       <c r="E406">
         <v>0.1</v>
@@ -32245,7 +32328,7 @@
         <v>287</v>
       </c>
       <c r="G406">
-        <v>6.2506999999999993E-2</v>
+        <v>6.1355E-2</v>
       </c>
       <c r="H406">
         <v>180</v>
@@ -32263,49 +32346,49 @@
         <v>40</v>
       </c>
       <c r="M406">
-        <v>35.019632000000001</v>
+        <v>35.002257</v>
       </c>
       <c r="N406">
-        <v>89.790706999999998</v>
+        <v>89.775952000000004</v>
       </c>
       <c r="O406">
         <v>25</v>
       </c>
       <c r="P406">
-        <v>3.6209999999999999E-2</v>
+        <v>3.5196999999999999E-2</v>
       </c>
       <c r="Q406">
-        <v>0.144568</v>
+        <v>0.14471999999999999</v>
       </c>
       <c r="R406">
-        <v>0.81922099999999998</v>
+        <v>0.82008199999999998</v>
       </c>
       <c r="S406">
-        <v>-10793.040702</v>
+        <v>-11080.902619</v>
       </c>
       <c r="T406">
-        <v>176350.33597099999</v>
+        <v>174747.071669</v>
       </c>
       <c r="U406">
-        <v>69092.880864999999</v>
+        <v>73035.965695999999</v>
       </c>
       <c r="V406">
-        <v>33.518452000000003</v>
+        <v>33.573515999999998</v>
       </c>
       <c r="W406">
-        <v>49.893824000000002</v>
+        <v>49.959420999999999</v>
       </c>
       <c r="X406">
-        <v>26.628795</v>
+        <v>26.106241000000001</v>
       </c>
       <c r="Y406">
-        <v>15.998042</v>
+        <v>16.537134999999999</v>
       </c>
       <c r="Z406">
-        <v>33.906309999999998</v>
+        <v>35.310056000000003</v>
       </c>
       <c r="AA406">
-        <v>-9.7807000000000005E-2</v>
+        <v>-9.8048999999999997E-2</v>
       </c>
     </row>
     <row r="407" spans="1:27" x14ac:dyDescent="0.35">
@@ -32313,13 +32396,13 @@
         <v>287</v>
       </c>
       <c r="B407">
-        <v>106000</v>
+        <v>110000</v>
       </c>
       <c r="C407">
         <v>861</v>
       </c>
       <c r="D407">
-        <v>106000</v>
+        <v>110000</v>
       </c>
       <c r="E407">
         <v>0.1</v>
@@ -32328,7 +32411,7 @@
         <v>287</v>
       </c>
       <c r="G407">
-        <v>6.0713999999999997E-2</v>
+        <v>5.9325999999999997E-2</v>
       </c>
       <c r="H407">
         <v>180</v>
@@ -32346,49 +32429,49 @@
         <v>40</v>
       </c>
       <c r="M407">
-        <v>35.012256999999998</v>
+        <v>35.002746000000002</v>
       </c>
       <c r="N407">
-        <v>89.767812000000006</v>
+        <v>89.754478000000006</v>
       </c>
       <c r="O407">
         <v>25</v>
       </c>
       <c r="P407">
-        <v>3.4787999999999999E-2</v>
+        <v>3.3647999999999997E-2</v>
       </c>
       <c r="Q407">
-        <v>0.14478199999999999</v>
+        <v>0.144953</v>
       </c>
       <c r="R407">
-        <v>0.82042999999999999</v>
+        <v>0.82139899999999999</v>
       </c>
       <c r="S407">
-        <v>-11405.690839000001</v>
+        <v>-11830.733292000001</v>
       </c>
       <c r="T407">
-        <v>174679.10399800001</v>
+        <v>173596.75700400001</v>
       </c>
       <c r="U407">
-        <v>74392.285585999998</v>
+        <v>77914.846653999994</v>
       </c>
       <c r="V407">
-        <v>33.592737</v>
+        <v>33.647959</v>
       </c>
       <c r="W407">
-        <v>49.980331999999997</v>
+        <v>50.048682999999997</v>
       </c>
       <c r="X407">
-        <v>25.820681</v>
+        <v>25.197534999999998</v>
       </c>
       <c r="Y407">
-        <v>16.833064</v>
+        <v>17.399940999999998</v>
       </c>
       <c r="Z407">
-        <v>35.993276999999999</v>
+        <v>37.492589000000002</v>
       </c>
       <c r="AA407">
-        <v>-9.8921999999999996E-2</v>
+        <v>-0.102283</v>
       </c>
     </row>
     <row r="408" spans="1:27" x14ac:dyDescent="0.35">
@@ -32396,13 +32479,13 @@
         <v>287</v>
       </c>
       <c r="B408">
-        <v>112000</v>
+        <v>116000</v>
       </c>
       <c r="C408">
         <v>861</v>
       </c>
       <c r="D408">
-        <v>112000</v>
+        <v>116000</v>
       </c>
       <c r="E408">
         <v>0.1</v>
@@ -32411,7 +32494,7 @@
         <v>287</v>
       </c>
       <c r="G408">
-        <v>5.8631999999999997E-2</v>
+        <v>5.7253999999999999E-2</v>
       </c>
       <c r="H408">
         <v>180</v>
@@ -32429,49 +32512,49 @@
         <v>40</v>
       </c>
       <c r="M408">
-        <v>35.003115000000001</v>
+        <v>35.003157000000002</v>
       </c>
       <c r="N408">
-        <v>89.746872999999994</v>
+        <v>89.734094999999996</v>
       </c>
       <c r="O408">
         <v>25</v>
       </c>
       <c r="P408">
-        <v>3.3105000000000002E-2</v>
+        <v>3.2028000000000001E-2</v>
       </c>
       <c r="Q408">
-        <v>0.145034</v>
+        <v>0.14519599999999999</v>
       </c>
       <c r="R408">
-        <v>0.82186099999999995</v>
+        <v>0.82277599999999995</v>
       </c>
       <c r="S408">
-        <v>-12054.688426000001</v>
+        <v>-12474.721449000001</v>
       </c>
       <c r="T408">
-        <v>173083.07619600001</v>
+        <v>171951.863064</v>
       </c>
       <c r="U408">
-        <v>79563.642261999994</v>
+        <v>82917.279704999994</v>
       </c>
       <c r="V408">
-        <v>33.675063000000002</v>
+        <v>33.728492000000003</v>
       </c>
       <c r="W408">
-        <v>50.081195000000001</v>
+        <v>50.146375999999997</v>
       </c>
       <c r="X408">
-        <v>24.886409</v>
+        <v>24.269583999999998</v>
       </c>
       <c r="Y408">
-        <v>17.669978</v>
+        <v>18.437904</v>
       </c>
       <c r="Z408">
-        <v>38.203201</v>
+        <v>40.131829000000003</v>
       </c>
       <c r="AA408">
-        <v>-0.103949</v>
+        <v>-0.107113</v>
       </c>
     </row>
     <row r="409" spans="1:27" x14ac:dyDescent="0.35">
@@ -32479,13 +32562,13 @@
         <v>287</v>
       </c>
       <c r="B409">
-        <v>118000</v>
+        <v>122000</v>
       </c>
       <c r="C409">
         <v>861</v>
       </c>
       <c r="D409">
-        <v>118000</v>
+        <v>122000</v>
       </c>
       <c r="E409">
         <v>0.1</v>
@@ -32494,7 +32577,7 @@
         <v>287</v>
       </c>
       <c r="G409">
-        <v>5.6600999999999999E-2</v>
+        <v>5.5271000000000001E-2</v>
       </c>
       <c r="H409">
         <v>180</v>
@@ -32512,49 +32595,49 @@
         <v>40</v>
       </c>
       <c r="M409">
-        <v>35.013626000000002</v>
+        <v>35.003559000000003</v>
       </c>
       <c r="N409">
-        <v>89.727276000000003</v>
+        <v>89.714878999999996</v>
       </c>
       <c r="O409">
         <v>25</v>
       </c>
       <c r="P409">
-        <v>3.1572999999999997E-2</v>
+        <v>3.0439000000000001E-2</v>
       </c>
       <c r="Q409">
-        <v>0.145264</v>
+        <v>0.14543400000000001</v>
       </c>
       <c r="R409">
-        <v>0.82316299999999998</v>
+        <v>0.82412600000000003</v>
       </c>
       <c r="S409">
-        <v>-12809.459632</v>
+        <v>-13330.126754999999</v>
       </c>
       <c r="T409">
-        <v>171358.16383599999</v>
+        <v>170008.05805200001</v>
       </c>
       <c r="U409">
-        <v>84568.864096999998</v>
+        <v>88219.281124999994</v>
       </c>
       <c r="V409">
-        <v>33.751480999999998</v>
+        <v>33.808323000000001</v>
       </c>
       <c r="W409">
-        <v>50.174348000000002</v>
+        <v>50.246040000000001</v>
       </c>
       <c r="X409">
-        <v>23.978154</v>
+        <v>23.381292999999999</v>
       </c>
       <c r="Y409">
-        <v>18.643284999999999</v>
+        <v>19.297198999999999</v>
       </c>
       <c r="Z409">
-        <v>40.668073</v>
+        <v>42.444980000000001</v>
       </c>
       <c r="AA409">
-        <v>-0.108168</v>
+        <v>-0.11071400000000001</v>
       </c>
     </row>
     <row r="410" spans="1:27" x14ac:dyDescent="0.35">
@@ -32562,13 +32645,13 @@
         <v>287</v>
       </c>
       <c r="B410">
-        <v>124000</v>
+        <v>128000</v>
       </c>
       <c r="C410">
         <v>861</v>
       </c>
       <c r="D410">
-        <v>124000</v>
+        <v>128000</v>
       </c>
       <c r="E410">
         <v>0.1</v>
@@ -32577,7 +32660,7 @@
         <v>287</v>
       </c>
       <c r="G410">
-        <v>5.4436999999999999E-2</v>
+        <v>5.2770999999999998E-2</v>
       </c>
       <c r="H410">
         <v>180</v>
@@ -32595,49 +32678,49 @@
         <v>40</v>
       </c>
       <c r="M410">
-        <v>35.004441999999997</v>
+        <v>34.999327000000001</v>
       </c>
       <c r="N410">
-        <v>89.705983000000003</v>
+        <v>89.694272999999995</v>
       </c>
       <c r="O410">
         <v>25</v>
       </c>
       <c r="P410">
-        <v>2.9767999999999999E-2</v>
+        <v>2.8441000000000001E-2</v>
       </c>
       <c r="Q410">
-        <v>0.145535</v>
+        <v>0.145734</v>
       </c>
       <c r="R410">
-        <v>0.82469700000000001</v>
+        <v>0.82582500000000003</v>
       </c>
       <c r="S410">
-        <v>-13543.448003</v>
+        <v>-14114.016621999999</v>
       </c>
       <c r="T410">
-        <v>169849.00768099999</v>
+        <v>168446.77422699999</v>
       </c>
       <c r="U410">
-        <v>89509.494531000004</v>
+        <v>93173.684393000003</v>
       </c>
       <c r="V410">
-        <v>33.838828999999997</v>
+        <v>33.90072</v>
       </c>
       <c r="W410">
-        <v>50.282522</v>
+        <v>50.363791999999997</v>
       </c>
       <c r="X410">
-        <v>23.012706000000001</v>
+        <v>22.271180000000001</v>
       </c>
       <c r="Y410">
-        <v>19.542477999999999</v>
+        <v>20.390540999999999</v>
       </c>
       <c r="Z410">
-        <v>43.183298999999998</v>
+        <v>45.459049</v>
       </c>
       <c r="AA410">
-        <v>-0.114161</v>
+        <v>-0.12119099999999999</v>
       </c>
     </row>
     <row r="411" spans="1:27" x14ac:dyDescent="0.35">
@@ -32645,13 +32728,13 @@
         <v>287</v>
       </c>
       <c r="B411">
-        <v>130000</v>
+        <v>134000</v>
       </c>
       <c r="C411">
         <v>861</v>
       </c>
       <c r="D411">
-        <v>130000</v>
+        <v>134000</v>
       </c>
       <c r="E411">
         <v>0.1</v>
@@ -32660,7 +32743,7 @@
         <v>287</v>
       </c>
       <c r="G411">
-        <v>5.2250999999999999E-2</v>
+        <v>5.0708000000000003E-2</v>
       </c>
       <c r="H411">
         <v>180</v>
@@ -32678,49 +32761,49 @@
         <v>40</v>
       </c>
       <c r="M411">
-        <v>35.015692000000001</v>
+        <v>35.004497000000001</v>
       </c>
       <c r="N411">
-        <v>89.683139999999995</v>
+        <v>89.669805999999994</v>
       </c>
       <c r="O411">
         <v>25</v>
       </c>
       <c r="P411">
-        <v>2.8032000000000001E-2</v>
+        <v>2.6682999999999998E-2</v>
       </c>
       <c r="Q411">
-        <v>0.14579500000000001</v>
+        <v>0.14599799999999999</v>
       </c>
       <c r="R411">
-        <v>0.82617300000000005</v>
+        <v>0.82732000000000006</v>
       </c>
       <c r="S411">
-        <v>-14436.674653</v>
+        <v>-15058.838406999999</v>
       </c>
       <c r="T411">
-        <v>167918.77198300001</v>
+        <v>166958.93249199999</v>
       </c>
       <c r="U411">
-        <v>94659.964743000004</v>
+        <v>97757.801720999996</v>
       </c>
       <c r="V411">
-        <v>33.924385000000001</v>
+        <v>33.984560000000002</v>
       </c>
       <c r="W411">
-        <v>50.388964999999999</v>
+        <v>50.469372999999997</v>
       </c>
       <c r="X411">
-        <v>22.041205999999999</v>
+        <v>21.35707</v>
       </c>
       <c r="Y411">
-        <v>20.580248999999998</v>
+        <v>21.346150999999999</v>
       </c>
       <c r="Z411">
-        <v>46.007632000000001</v>
+        <v>48.234212999999997</v>
       </c>
       <c r="AA411">
-        <v>-0.120341</v>
+        <v>-0.12559200000000001</v>
       </c>
     </row>
     <row r="412" spans="1:27" x14ac:dyDescent="0.35">
@@ -32728,13 +32811,13 @@
         <v>287</v>
       </c>
       <c r="B412">
-        <v>136000</v>
+        <v>140000</v>
       </c>
       <c r="C412">
         <v>861</v>
       </c>
       <c r="D412">
-        <v>136000</v>
+        <v>140000</v>
       </c>
       <c r="E412">
         <v>0.1</v>
@@ -32743,7 +32826,7 @@
         <v>287</v>
       </c>
       <c r="G412">
-        <v>4.9950000000000001E-2</v>
+        <v>4.8753999999999999E-2</v>
       </c>
       <c r="H412">
         <v>180</v>
@@ -32761,49 +32844,49 @@
         <v>40</v>
       </c>
       <c r="M412">
-        <v>35.004758000000002</v>
+        <v>35.015498999999998</v>
       </c>
       <c r="N412">
-        <v>89.659813999999997</v>
+        <v>89.638806000000002</v>
       </c>
       <c r="O412">
         <v>25</v>
       </c>
       <c r="P412">
-        <v>2.6037999999999999E-2</v>
+        <v>2.5033E-2</v>
       </c>
       <c r="Q412">
-        <v>0.146094</v>
+        <v>0.14624500000000001</v>
       </c>
       <c r="R412">
-        <v>0.82786800000000005</v>
+        <v>0.82872199999999996</v>
       </c>
       <c r="S412">
-        <v>-15459.934458</v>
+        <v>-16309.476920999999</v>
       </c>
       <c r="T412">
-        <v>166251.87699300001</v>
+        <v>165147.204772</v>
       </c>
       <c r="U412">
-        <v>99587.934534999993</v>
+        <v>102462.986546</v>
       </c>
       <c r="V412">
-        <v>34.016072000000001</v>
+        <v>34.065753000000001</v>
       </c>
       <c r="W412">
-        <v>50.508980000000001</v>
+        <v>50.571016</v>
       </c>
       <c r="X412">
-        <v>21.022174</v>
+        <v>20.493974000000001</v>
       </c>
       <c r="Y412">
-        <v>21.662901000000002</v>
+        <v>22.183986999999998</v>
       </c>
       <c r="Z412">
-        <v>49.194820999999997</v>
+        <v>50.766478999999997</v>
       </c>
       <c r="AA412">
-        <v>-0.127995</v>
+        <v>-0.128412</v>
       </c>
     </row>
     <row r="413" spans="1:27" x14ac:dyDescent="0.35">
@@ -32811,13 +32894,13 @@
         <v>287</v>
       </c>
       <c r="B413">
-        <v>142000</v>
+        <v>146000</v>
       </c>
       <c r="C413">
         <v>861</v>
       </c>
       <c r="D413">
-        <v>142000</v>
+        <v>146000</v>
       </c>
       <c r="E413">
         <v>0.1</v>
@@ -32826,7 +32909,7 @@
         <v>287</v>
       </c>
       <c r="G413">
-        <v>4.7967000000000003E-2</v>
+        <v>4.6413000000000003E-2</v>
       </c>
       <c r="H413">
         <v>180</v>
@@ -32844,49 +32927,49 @@
         <v>40</v>
       </c>
       <c r="M413">
-        <v>34.999994000000001</v>
+        <v>35.006107999999998</v>
       </c>
       <c r="N413">
-        <v>89.628969999999995</v>
+        <v>89.603684000000001</v>
       </c>
       <c r="O413">
         <v>25</v>
       </c>
       <c r="P413">
-        <v>2.4317999999999999E-2</v>
+        <v>2.2884000000000002E-2</v>
       </c>
       <c r="Q413">
-        <v>0.14635200000000001</v>
+        <v>0.146567</v>
       </c>
       <c r="R413">
-        <v>0.82933000000000001</v>
+        <v>0.83054899999999998</v>
       </c>
       <c r="S413">
-        <v>-16861.900592999998</v>
+        <v>-18033.286080999998</v>
       </c>
       <c r="T413">
-        <v>164664.80016399999</v>
+        <v>163692.468972</v>
       </c>
       <c r="U413">
-        <v>103944.19792599999</v>
+        <v>106788.62626200001</v>
       </c>
       <c r="V413">
-        <v>34.095374</v>
+        <v>34.157389000000002</v>
       </c>
       <c r="W413">
-        <v>50.613548000000002</v>
+        <v>50.698593000000002</v>
       </c>
       <c r="X413">
-        <v>20.146764999999998</v>
+        <v>19.462886999999998</v>
       </c>
       <c r="Y413">
-        <v>22.491350000000001</v>
+        <v>23.145752000000002</v>
       </c>
       <c r="Z413">
-        <v>51.78884</v>
+        <v>53.980316999999999</v>
       </c>
       <c r="AA413">
-        <v>-0.13119700000000001</v>
+        <v>-0.13644000000000001</v>
       </c>
     </row>
     <row r="414" spans="1:27" x14ac:dyDescent="0.35">
@@ -32894,13 +32977,13 @@
         <v>287</v>
       </c>
       <c r="B414">
-        <v>148000</v>
+        <v>152000</v>
       </c>
       <c r="C414">
         <v>861</v>
       </c>
       <c r="D414">
-        <v>148000</v>
+        <v>152000</v>
       </c>
       <c r="E414">
         <v>0.1</v>
@@ -32909,7 +32992,7 @@
         <v>287</v>
       </c>
       <c r="G414">
-        <v>4.5953000000000001E-2</v>
+        <v>4.4776999999999997E-2</v>
       </c>
       <c r="H414">
         <v>180</v>
@@ -32927,49 +33010,49 @@
         <v>40</v>
       </c>
       <c r="M414">
-        <v>34.999836000000002</v>
+        <v>35.005944</v>
       </c>
       <c r="N414">
-        <v>89.584258000000005</v>
+        <v>89.547054000000003</v>
       </c>
       <c r="O414">
         <v>25</v>
       </c>
       <c r="P414">
-        <v>2.2499000000000002E-2</v>
+        <v>2.1359E-2</v>
       </c>
       <c r="Q414">
-        <v>0.14662500000000001</v>
+        <v>0.14679600000000001</v>
       </c>
       <c r="R414">
-        <v>0.83087599999999995</v>
+        <v>0.83184499999999995</v>
       </c>
       <c r="S414">
-        <v>-18790.800888999998</v>
+        <v>-20268.149690999999</v>
       </c>
       <c r="T414">
-        <v>163096.38726399999</v>
+        <v>161967.117727</v>
       </c>
       <c r="U414">
-        <v>108103.821064</v>
+        <v>110618.113214</v>
       </c>
       <c r="V414">
-        <v>34.178207999999998</v>
+        <v>34.232816</v>
       </c>
       <c r="W414">
-        <v>50.723646000000002</v>
+        <v>50.794392000000002</v>
       </c>
       <c r="X414">
-        <v>19.260190999999999</v>
+        <v>18.743019</v>
       </c>
       <c r="Y414">
-        <v>23.501256999999999</v>
+        <v>23.880884999999999</v>
       </c>
       <c r="Z414">
-        <v>54.974620000000002</v>
+        <v>56.475931000000003</v>
       </c>
       <c r="AA414">
-        <v>-0.134744</v>
+        <v>-0.13481899999999999</v>
       </c>
     </row>
     <row r="415" spans="1:27" x14ac:dyDescent="0.35">
@@ -32977,13 +33060,13 @@
         <v>287</v>
       </c>
       <c r="B415">
-        <v>154000</v>
+        <v>158000</v>
       </c>
       <c r="C415">
         <v>861</v>
       </c>
       <c r="D415">
-        <v>154000</v>
+        <v>158000</v>
       </c>
       <c r="E415">
         <v>0.1</v>
@@ -32992,7 +33075,7 @@
         <v>287</v>
       </c>
       <c r="G415">
-        <v>4.4474E-2</v>
+        <v>4.3727000000000002E-2</v>
       </c>
       <c r="H415">
         <v>180</v>
@@ -33010,49 +33093,49 @@
         <v>40</v>
       </c>
       <c r="M415">
-        <v>35.003484999999998</v>
+        <v>35.011690999999999</v>
       </c>
       <c r="N415">
-        <v>89.517263</v>
+        <v>89.472465</v>
       </c>
       <c r="O415">
         <v>25</v>
       </c>
       <c r="P415">
-        <v>2.1089E-2</v>
+        <v>2.0323000000000001E-2</v>
       </c>
       <c r="Q415">
-        <v>0.146837</v>
+        <v>0.146951</v>
       </c>
       <c r="R415">
-        <v>0.83207500000000001</v>
+        <v>0.83272500000000005</v>
       </c>
       <c r="S415">
-        <v>-21459.288475000001</v>
+        <v>-23649.765619000002</v>
       </c>
       <c r="T415">
-        <v>161841.01626</v>
+        <v>160969.57862099999</v>
       </c>
       <c r="U415">
-        <v>111314.54552499999</v>
+        <v>113181.352063</v>
       </c>
       <c r="V415">
-        <v>34.246422000000003</v>
+        <v>34.279437000000001</v>
       </c>
       <c r="W415">
-        <v>50.809151999999997</v>
+        <v>50.857712999999997</v>
       </c>
       <c r="X415">
-        <v>18.612003999999999</v>
+        <v>18.283071</v>
       </c>
       <c r="Y415">
-        <v>24.004370999999999</v>
+        <v>24.358073999999998</v>
       </c>
       <c r="Z415">
-        <v>56.905515999999999</v>
+        <v>58.20147</v>
       </c>
       <c r="AA415">
-        <v>-0.13090199999999999</v>
+        <v>-0.125142</v>
       </c>
     </row>
     <row r="416" spans="1:27" x14ac:dyDescent="0.35">
@@ -33060,13 +33143,13 @@
         <v>287</v>
       </c>
       <c r="B416">
-        <v>160000</v>
+        <v>164000</v>
       </c>
       <c r="C416">
         <v>861</v>
       </c>
       <c r="D416">
-        <v>160000</v>
+        <v>164000</v>
       </c>
       <c r="E416">
         <v>0.1</v>
@@ -33075,7 +33158,7 @@
         <v>287</v>
       </c>
       <c r="G416">
-        <v>4.3324000000000001E-2</v>
+        <v>4.2655999999999999E-2</v>
       </c>
       <c r="H416">
         <v>180</v>
@@ -33093,49 +33176,49 @@
         <v>40</v>
       </c>
       <c r="M416">
-        <v>35.012585000000001</v>
+        <v>35.012008999999999</v>
       </c>
       <c r="N416">
-        <v>89.444111000000007</v>
+        <v>89.382390999999998</v>
       </c>
       <c r="O416">
         <v>25</v>
       </c>
       <c r="P416">
-        <v>1.9934E-2</v>
+        <v>1.9265999999999998E-2</v>
       </c>
       <c r="Q416">
-        <v>0.14701</v>
+        <v>0.14710999999999999</v>
       </c>
       <c r="R416">
-        <v>0.83305600000000002</v>
+        <v>0.83362400000000003</v>
       </c>
       <c r="S416">
-        <v>-24878.019461</v>
+        <v>-27656.123449999999</v>
       </c>
       <c r="T416">
-        <v>160603.05020299999</v>
+        <v>160115.59169100001</v>
       </c>
       <c r="U416">
-        <v>114007.761237</v>
+        <v>115264.331678</v>
       </c>
       <c r="V416">
-        <v>34.296967000000002</v>
+        <v>34.323889999999999</v>
       </c>
       <c r="W416">
-        <v>50.881447000000001</v>
+        <v>50.921322000000004</v>
       </c>
       <c r="X416">
-        <v>18.107127999999999</v>
+        <v>17.815269000000001</v>
       </c>
       <c r="Y416">
-        <v>24.493354</v>
+        <v>24.875114</v>
       </c>
       <c r="Z416">
-        <v>58.749642000000001</v>
+        <v>60.074750000000002</v>
       </c>
       <c r="AA416">
-        <v>-0.122617</v>
+        <v>-0.115707</v>
       </c>
     </row>
     <row r="417" spans="1:27" x14ac:dyDescent="0.35">
@@ -33143,13 +33226,13 @@
         <v>287</v>
       </c>
       <c r="B417">
-        <v>166000</v>
+        <v>170000</v>
       </c>
       <c r="C417">
         <v>861</v>
       </c>
       <c r="D417">
-        <v>166000</v>
+        <v>170000</v>
       </c>
       <c r="E417">
         <v>0.1</v>
@@ -33158,7 +33241,7 @@
         <v>287</v>
       </c>
       <c r="G417">
-        <v>4.2318000000000001E-2</v>
+        <v>4.1812000000000002E-2</v>
       </c>
       <c r="H417">
         <v>180</v>
@@ -33176,132 +33259,132 @@
         <v>40</v>
       </c>
       <c r="M417">
-        <v>35.011541999999999</v>
+        <v>35.001888999999998</v>
       </c>
       <c r="N417">
-        <v>89.340655999999996</v>
+        <v>89.263841999999997</v>
       </c>
       <c r="O417">
         <v>25</v>
       </c>
       <c r="P417">
-        <v>1.8928E-2</v>
+        <v>1.8386E-2</v>
       </c>
       <c r="Q417">
-        <v>0.14716099999999999</v>
+        <v>0.14724200000000001</v>
       </c>
       <c r="R417">
-        <v>0.83391099999999996</v>
+        <v>0.83437099999999997</v>
       </c>
       <c r="S417">
-        <v>-29084.423846999998</v>
+        <v>-32151.358345000001</v>
       </c>
       <c r="T417">
-        <v>159854.893098</v>
+        <v>160213.39095900001</v>
       </c>
       <c r="U417">
-        <v>115884.946484</v>
+        <v>116237.132598</v>
       </c>
       <c r="V417">
-        <v>34.338527999999997</v>
+        <v>34.363059</v>
       </c>
       <c r="W417">
-        <v>50.941588000000003</v>
+        <v>50.968797000000002</v>
       </c>
       <c r="X417">
-        <v>17.667466000000001</v>
+        <v>17.447009999999999</v>
       </c>
       <c r="Y417">
-        <v>24.992443000000002</v>
+        <v>25.118853000000001</v>
       </c>
       <c r="Z417">
-        <v>60.569519999999997</v>
+        <v>60.074750000000002</v>
       </c>
       <c r="AA417">
-        <v>-0.11230999999999999</v>
-      </c>
-    </row>
-    <row r="418" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A418">
+        <v>-0.103187</v>
+      </c>
+    </row>
+    <row r="418" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A418" s="4">
         <v>287</v>
       </c>
-      <c r="B418">
-        <v>172000</v>
-      </c>
-      <c r="C418">
+      <c r="B418" s="4">
+        <v>176000</v>
+      </c>
+      <c r="C418" s="4">
         <v>861</v>
       </c>
-      <c r="D418">
-        <v>172000</v>
-      </c>
-      <c r="E418">
-        <v>0.1</v>
-      </c>
-      <c r="F418">
+      <c r="D418" s="4">
+        <v>170000</v>
+      </c>
+      <c r="E418" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="F418" s="4">
         <v>287</v>
       </c>
-      <c r="G418">
-        <v>4.1565999999999999E-2</v>
-      </c>
-      <c r="H418">
-        <v>180</v>
-      </c>
-      <c r="I418">
-        <v>180</v>
-      </c>
-      <c r="J418">
-        <v>170</v>
-      </c>
-      <c r="K418">
-        <v>170</v>
-      </c>
-      <c r="L418">
-        <v>40</v>
-      </c>
-      <c r="M418">
-        <v>35.009974</v>
-      </c>
-      <c r="N418">
-        <v>89.226603999999995</v>
-      </c>
-      <c r="O418">
-        <v>25</v>
-      </c>
-      <c r="P418">
-        <v>1.8148999999999998E-2</v>
-      </c>
-      <c r="Q418">
-        <v>0.14727799999999999</v>
-      </c>
-      <c r="R418">
-        <v>0.83457300000000001</v>
-      </c>
-      <c r="S418">
-        <v>-33787.580203999998</v>
-      </c>
-      <c r="T418">
-        <v>159945.017666</v>
-      </c>
-      <c r="U418">
-        <v>116773.865714</v>
-      </c>
-      <c r="V418">
-        <v>34.373184000000002</v>
-      </c>
-      <c r="W418">
-        <v>50.983562999999997</v>
-      </c>
-      <c r="X418">
-        <v>17.339931</v>
-      </c>
-      <c r="Y418">
-        <v>25.372579999999999</v>
-      </c>
-      <c r="Z418">
-        <v>62.009915999999997</v>
-      </c>
-      <c r="AA418">
-        <v>-9.8528000000000004E-2</v>
+      <c r="G418" s="4">
+        <v>4.1812000000000002E-2</v>
+      </c>
+      <c r="H418" s="4">
+        <v>180</v>
+      </c>
+      <c r="I418" s="4">
+        <v>180</v>
+      </c>
+      <c r="J418" s="4">
+        <v>170</v>
+      </c>
+      <c r="K418" s="4">
+        <v>170</v>
+      </c>
+      <c r="L418" s="4">
+        <v>40</v>
+      </c>
+      <c r="M418" s="4">
+        <v>35.001888999999998</v>
+      </c>
+      <c r="N418" s="4">
+        <v>89.263841999999997</v>
+      </c>
+      <c r="O418" s="4">
+        <v>25</v>
+      </c>
+      <c r="P418" s="4">
+        <v>1.8386E-2</v>
+      </c>
+      <c r="Q418" s="4">
+        <v>0.14724200000000001</v>
+      </c>
+      <c r="R418" s="4">
+        <v>0.83437099999999997</v>
+      </c>
+      <c r="S418" s="4">
+        <v>-32151.358345000001</v>
+      </c>
+      <c r="T418" s="4">
+        <v>160213.39095900001</v>
+      </c>
+      <c r="U418" s="4">
+        <v>116237.132598</v>
+      </c>
+      <c r="V418" s="4">
+        <v>34.363059</v>
+      </c>
+      <c r="W418" s="4">
+        <v>50.968797000000002</v>
+      </c>
+      <c r="X418" s="4">
+        <v>17.447009999999999</v>
+      </c>
+      <c r="Y418" s="4">
+        <v>25.118853000000001</v>
+      </c>
+      <c r="Z418" s="4">
+        <v>60.074750000000002</v>
+      </c>
+      <c r="AA418" s="4">
+        <v>-0.103187</v>
       </c>
     </row>
     <row r="419" spans="1:27" x14ac:dyDescent="0.35">
@@ -33309,13 +33392,13 @@
         <v>287</v>
       </c>
       <c r="B419">
-        <v>178000</v>
+        <v>182000</v>
       </c>
       <c r="C419">
         <v>861</v>
       </c>
       <c r="D419">
-        <v>178000</v>
+        <v>182000</v>
       </c>
       <c r="E419">
         <v>0.1</v>
@@ -33324,7 +33407,7 @@
         <v>287</v>
       </c>
       <c r="G419">
-        <v>4.0913999999999999E-2</v>
+        <v>4.0541000000000001E-2</v>
       </c>
       <c r="H419">
         <v>180</v>
@@ -33342,49 +33425,49 @@
         <v>40</v>
       </c>
       <c r="M419">
-        <v>35.005828000000001</v>
+        <v>35.013717</v>
       </c>
       <c r="N419">
-        <v>89.130870000000002</v>
+        <v>89.055944999999994</v>
       </c>
       <c r="O419">
         <v>25</v>
       </c>
       <c r="P419">
-        <v>1.7507999999999999E-2</v>
+        <v>1.7083999999999998E-2</v>
       </c>
       <c r="Q419">
-        <v>0.147374</v>
+        <v>0.14743700000000001</v>
       </c>
       <c r="R419">
-        <v>0.83511800000000003</v>
+        <v>0.83547899999999997</v>
       </c>
       <c r="S419">
-        <v>-38240.410253000002</v>
+        <v>-41665.217663000003</v>
       </c>
       <c r="T419">
-        <v>158898.628708</v>
+        <v>158471.33293599999</v>
       </c>
       <c r="U419">
-        <v>118481.33777300001</v>
+        <v>119340.093798</v>
       </c>
       <c r="V419">
-        <v>34.400312999999997</v>
+        <v>34.417031999999999</v>
       </c>
       <c r="W419">
-        <v>51.025405999999997</v>
+        <v>51.051720000000003</v>
       </c>
       <c r="X419">
-        <v>17.055855999999999</v>
+        <v>16.893190000000001</v>
       </c>
       <c r="Y419">
-        <v>25.669314</v>
+        <v>25.701740999999998</v>
       </c>
       <c r="Z419">
-        <v>63.152101999999999</v>
+        <v>63.553125000000001</v>
       </c>
       <c r="AA419">
-        <v>-8.3398E-2</v>
+        <v>-7.2483000000000006E-2</v>
       </c>
     </row>
     <row r="420" spans="1:27" x14ac:dyDescent="0.35">
@@ -33392,13 +33475,13 @@
         <v>287</v>
       </c>
       <c r="B420">
-        <v>184000</v>
+        <v>188000</v>
       </c>
       <c r="C420">
         <v>861</v>
       </c>
       <c r="D420">
-        <v>184000</v>
+        <v>188000</v>
       </c>
       <c r="E420">
         <v>0.1</v>
@@ -33407,7 +33490,7 @@
         <v>287</v>
       </c>
       <c r="G420">
-        <v>4.0397000000000002E-2</v>
+        <v>3.9983999999999999E-2</v>
       </c>
       <c r="H420">
         <v>180</v>
@@ -33425,49 +33508,49 @@
         <v>40</v>
       </c>
       <c r="M420">
-        <v>35.008662000000001</v>
+        <v>35.005806</v>
       </c>
       <c r="N420">
-        <v>89.004363999999995</v>
+        <v>88.926704000000001</v>
       </c>
       <c r="O420">
         <v>25</v>
       </c>
       <c r="P420">
-        <v>1.6930000000000001E-2</v>
+        <v>1.6482E-2</v>
       </c>
       <c r="Q420">
-        <v>0.14746000000000001</v>
+        <v>0.14752799999999999</v>
       </c>
       <c r="R420">
-        <v>0.83560900000000005</v>
+        <v>0.83599100000000004</v>
       </c>
       <c r="S420">
-        <v>-43474.793986999997</v>
+        <v>-46852.566072000001</v>
       </c>
       <c r="T420">
-        <v>158962.53247500001</v>
+        <v>158535.71710099999</v>
       </c>
       <c r="U420">
-        <v>119120.127441</v>
+        <v>119963.74980999999</v>
       </c>
       <c r="V420">
-        <v>34.427588999999998</v>
+        <v>34.448689999999999</v>
       </c>
       <c r="W420">
-        <v>51.056477000000001</v>
+        <v>51.084015000000001</v>
       </c>
       <c r="X420">
-        <v>16.831126000000001</v>
+        <v>16.651558999999999</v>
       </c>
       <c r="Y420">
-        <v>25.864991</v>
+        <v>25.935389000000001</v>
       </c>
       <c r="Z420">
-        <v>64.067989999999995</v>
+        <v>64.576059000000001</v>
       </c>
       <c r="AA420">
-        <v>-6.6428000000000001E-2</v>
+        <v>-5.6037999999999998E-2</v>
       </c>
     </row>
     <row r="421" spans="1:27" x14ac:dyDescent="0.35">
@@ -33475,13 +33558,13 @@
         <v>287</v>
       </c>
       <c r="B421">
-        <v>190000</v>
+        <v>194000</v>
       </c>
       <c r="C421">
         <v>861</v>
       </c>
       <c r="D421">
-        <v>190000</v>
+        <v>194000</v>
       </c>
       <c r="E421">
         <v>0.1</v>
@@ -33490,7 +33573,7 @@
         <v>287</v>
       </c>
       <c r="G421">
-        <v>3.9814000000000002E-2</v>
+        <v>3.9678999999999999E-2</v>
       </c>
       <c r="H421">
         <v>180</v>
@@ -33508,49 +33591,49 @@
         <v>40</v>
       </c>
       <c r="M421">
-        <v>35.005975999999997</v>
+        <v>35.007190000000001</v>
       </c>
       <c r="N421">
-        <v>88.890426000000005</v>
+        <v>88.831271000000001</v>
       </c>
       <c r="O421">
         <v>25</v>
       </c>
       <c r="P421">
-        <v>1.6326E-2</v>
+        <v>1.6126000000000001E-2</v>
       </c>
       <c r="Q421">
-        <v>0.14755099999999999</v>
+        <v>0.14758099999999999</v>
       </c>
       <c r="R421">
-        <v>0.83612299999999995</v>
+        <v>0.83629299999999995</v>
       </c>
       <c r="S421">
-        <v>-48283.716234</v>
+        <v>-51282.618167000001</v>
       </c>
       <c r="T421">
-        <v>158201.434824</v>
+        <v>158574.31225300001</v>
       </c>
       <c r="U421">
-        <v>120487.216507</v>
+        <v>120342.736093</v>
       </c>
       <c r="V421">
-        <v>34.459395000000001</v>
+        <v>34.459474</v>
       </c>
       <c r="W421">
-        <v>51.094558999999997</v>
+        <v>51.103090000000002</v>
       </c>
       <c r="X421">
-        <v>16.577856000000001</v>
+        <v>16.519188</v>
       </c>
       <c r="Y421">
-        <v>26.024961999999999</v>
+        <v>26.101479999999999</v>
       </c>
       <c r="Z421">
-        <v>64.897184999999993</v>
+        <v>65.276280999999997</v>
       </c>
       <c r="AA421">
-        <v>-5.0344E-2</v>
+        <v>-3.6205000000000001E-2</v>
       </c>
     </row>
     <row r="422" spans="1:27" x14ac:dyDescent="0.35">
@@ -33558,13 +33641,13 @@
         <v>287</v>
       </c>
       <c r="B422">
-        <v>196000</v>
+        <v>200000</v>
       </c>
       <c r="C422">
         <v>861</v>
       </c>
       <c r="D422">
-        <v>196000</v>
+        <v>200000</v>
       </c>
       <c r="E422">
         <v>0.1</v>
@@ -33573,7 +33656,7 @@
         <v>287</v>
       </c>
       <c r="G422">
-        <v>3.9523999999999997E-2</v>
+        <v>3.9253999999999997E-2</v>
       </c>
       <c r="H422">
         <v>180</v>
@@ -33591,49 +33674,49 @@
         <v>40</v>
       </c>
       <c r="M422">
-        <v>35.007061</v>
+        <v>35.007589000000003</v>
       </c>
       <c r="N422">
-        <v>88.792264000000003</v>
+        <v>88.691121999999993</v>
       </c>
       <c r="O422">
         <v>25</v>
       </c>
       <c r="P422">
-        <v>1.5990000000000001E-2</v>
+        <v>1.5709999999999998E-2</v>
       </c>
       <c r="Q422">
-        <v>0.14760200000000001</v>
+        <v>0.147644</v>
       </c>
       <c r="R422">
-        <v>0.83640899999999996</v>
+        <v>0.83664700000000003</v>
       </c>
       <c r="S422">
-        <v>-53019.300169000002</v>
+        <v>-57204.997891999999</v>
       </c>
       <c r="T422">
-        <v>158237.47900699999</v>
+        <v>157649.11227899999</v>
       </c>
       <c r="U422">
-        <v>120825.267752</v>
+        <v>121762.193339</v>
       </c>
       <c r="V422">
-        <v>34.466476</v>
+        <v>34.486901000000003</v>
       </c>
       <c r="W422">
-        <v>51.112589999999997</v>
+        <v>51.131960999999997</v>
       </c>
       <c r="X422">
-        <v>16.452003000000001</v>
+        <v>16.334693999999999</v>
       </c>
       <c r="Y422">
-        <v>26.176884999999999</v>
+        <v>26.342212</v>
       </c>
       <c r="Z422">
-        <v>65.548542999999995</v>
+        <v>66.170344</v>
       </c>
       <c r="AA422">
-        <v>-3.0308999999999999E-2</v>
+        <v>-1.7988000000000001E-2</v>
       </c>
     </row>
     <row r="423" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -33661,11 +33744,86 @@
       </c>
     </row>
     <row r="426" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A426" s="2">
+      <c r="A426" s="3">
         <v>300</v>
       </c>
-      <c r="B426" s="2">
+      <c r="B426">
         <v>98000</v>
+      </c>
+      <c r="C426">
+        <v>900</v>
+      </c>
+      <c r="D426">
+        <v>98000</v>
+      </c>
+      <c r="E426">
+        <v>0.1</v>
+      </c>
+      <c r="F426">
+        <v>300</v>
+      </c>
+      <c r="G426">
+        <v>6.5041000000000002E-2</v>
+      </c>
+      <c r="H426">
+        <v>180</v>
+      </c>
+      <c r="I426">
+        <v>180</v>
+      </c>
+      <c r="J426">
+        <v>170</v>
+      </c>
+      <c r="K426">
+        <v>170</v>
+      </c>
+      <c r="L426">
+        <v>40</v>
+      </c>
+      <c r="M426">
+        <v>35.001975000000002</v>
+      </c>
+      <c r="N426">
+        <v>89.812405999999996</v>
+      </c>
+      <c r="O426">
+        <v>25</v>
+      </c>
+      <c r="P426">
+        <v>3.7740999999999997E-2</v>
+      </c>
+      <c r="Q426">
+        <v>0.144339</v>
+      </c>
+      <c r="R426">
+        <v>0.81791999999999998</v>
+      </c>
+      <c r="S426">
+        <v>-10568.5326</v>
+      </c>
+      <c r="T426">
+        <v>186446.43422900001</v>
+      </c>
+      <c r="U426">
+        <v>66521.669429000001</v>
+      </c>
+      <c r="V426">
+        <v>34.955795000000002</v>
+      </c>
+      <c r="W426">
+        <v>52.060532000000002</v>
+      </c>
+      <c r="X426">
+        <v>29.026548999999999</v>
+      </c>
+      <c r="Y426">
+        <v>15.630153</v>
+      </c>
+      <c r="Z426">
+        <v>31.572407999999999</v>
+      </c>
+      <c r="AA426">
+        <v>-9.1347999999999999E-2</v>
       </c>
     </row>
     <row r="427" spans="1:27" x14ac:dyDescent="0.35">
@@ -33673,13 +33831,13 @@
         <v>300</v>
       </c>
       <c r="B427">
-        <v>100000</v>
+        <v>104000</v>
       </c>
       <c r="C427">
         <v>900</v>
       </c>
       <c r="D427">
-        <v>100000</v>
+        <v>104000</v>
       </c>
       <c r="E427">
         <v>0.1</v>
@@ -33688,7 +33846,7 @@
         <v>300</v>
       </c>
       <c r="G427">
-        <v>6.4257999999999996E-2</v>
+        <v>6.3129000000000005E-2</v>
       </c>
       <c r="H427">
         <v>180</v>
@@ -33706,49 +33864,49 @@
         <v>40</v>
       </c>
       <c r="M427">
-        <v>35.019979999999997</v>
+        <v>35.001834000000002</v>
       </c>
       <c r="N427">
-        <v>89.805580000000006</v>
+        <v>89.789506000000003</v>
       </c>
       <c r="O427">
         <v>25</v>
       </c>
       <c r="P427">
-        <v>3.7206000000000003E-2</v>
+        <v>3.6214999999999997E-2</v>
       </c>
       <c r="Q427">
-        <v>0.14441899999999999</v>
+        <v>0.144568</v>
       </c>
       <c r="R427">
-        <v>0.81837499999999996</v>
+        <v>0.81921699999999997</v>
       </c>
       <c r="S427">
-        <v>-10661.246445999999</v>
+        <v>-10983.630042999999</v>
       </c>
       <c r="T427">
-        <v>185641.167755</v>
+        <v>183908.14275200001</v>
       </c>
       <c r="U427">
-        <v>68404.528976999994</v>
+        <v>72513.849732999995</v>
       </c>
       <c r="V427">
-        <v>34.984281000000003</v>
+        <v>35.040934</v>
       </c>
       <c r="W427">
-        <v>52.093449999999997</v>
+        <v>52.160696000000002</v>
       </c>
       <c r="X427">
-        <v>28.659241999999999</v>
+        <v>28.122488000000001</v>
       </c>
       <c r="Y427">
-        <v>15.918844999999999</v>
+        <v>16.458566000000001</v>
       </c>
       <c r="Z427">
-        <v>32.229582999999998</v>
+        <v>33.563375000000001</v>
       </c>
       <c r="AA427">
-        <v>-9.4755000000000006E-2</v>
+        <v>-9.5436999999999994E-2</v>
       </c>
     </row>
     <row r="428" spans="1:27" x14ac:dyDescent="0.35">
@@ -33756,13 +33914,13 @@
         <v>300</v>
       </c>
       <c r="B428">
-        <v>106000</v>
+        <v>110000</v>
       </c>
       <c r="C428">
         <v>900</v>
       </c>
       <c r="D428">
-        <v>106000</v>
+        <v>110000</v>
       </c>
       <c r="E428">
         <v>0.1</v>
@@ -33771,7 +33929,7 @@
         <v>300</v>
       </c>
       <c r="G428">
-        <v>6.2559000000000003E-2</v>
+        <v>6.1359999999999998E-2</v>
       </c>
       <c r="H428">
         <v>180</v>
@@ -33789,49 +33947,49 @@
         <v>40</v>
       </c>
       <c r="M428">
-        <v>35.001826000000001</v>
+        <v>35.011324000000002</v>
       </c>
       <c r="N428">
-        <v>89.782587000000007</v>
+        <v>89.768417999999997</v>
       </c>
       <c r="O428">
         <v>25</v>
       </c>
       <c r="P428">
-        <v>3.5777000000000003E-2</v>
+        <v>3.4911999999999999E-2</v>
       </c>
       <c r="Q428">
-        <v>0.14463300000000001</v>
+        <v>0.144763</v>
       </c>
       <c r="R428">
-        <v>0.81959000000000004</v>
+        <v>0.82032499999999997</v>
       </c>
       <c r="S428">
-        <v>-11205.16972</v>
+        <v>-11767.222787000001</v>
       </c>
       <c r="T428">
-        <v>183377.35728200001</v>
+        <v>182884.94492099999</v>
       </c>
       <c r="U428">
-        <v>74211.916702000002</v>
+        <v>77205.572738999996</v>
       </c>
       <c r="V428">
-        <v>35.064461999999999</v>
+        <v>35.108147000000002</v>
       </c>
       <c r="W428">
-        <v>52.188372000000001</v>
+        <v>52.238494000000003</v>
       </c>
       <c r="X428">
-        <v>27.853702999999999</v>
+        <v>27.291664999999998</v>
       </c>
       <c r="Y428">
-        <v>16.712972000000001</v>
+        <v>17.295508000000002</v>
       </c>
       <c r="Z428">
-        <v>34.169584999999998</v>
+        <v>35.517431999999999</v>
       </c>
       <c r="AA428">
-        <v>-9.5791000000000001E-2</v>
+        <v>-9.7256999999999996E-2</v>
       </c>
     </row>
     <row r="429" spans="1:27" x14ac:dyDescent="0.35">
@@ -33839,13 +33997,13 @@
         <v>300</v>
       </c>
       <c r="B429">
-        <v>112000</v>
+        <v>116000</v>
       </c>
       <c r="C429">
         <v>900</v>
       </c>
       <c r="D429">
-        <v>112000</v>
+        <v>116000</v>
       </c>
       <c r="E429">
         <v>0.1</v>
@@ -33854,7 +34012,7 @@
         <v>300</v>
       </c>
       <c r="G429">
-        <v>6.0668E-2</v>
+        <v>5.9433E-2</v>
       </c>
       <c r="H429">
         <v>180</v>
@@ -33872,49 +34030,49 @@
         <v>40</v>
       </c>
       <c r="M429">
-        <v>35.012179000000003</v>
+        <v>35.013179999999998</v>
       </c>
       <c r="N429">
-        <v>89.763031999999995</v>
+        <v>89.749122999999997</v>
       </c>
       <c r="O429">
         <v>25</v>
       </c>
       <c r="P429">
-        <v>3.4373000000000001E-2</v>
+        <v>3.3397999999999997E-2</v>
       </c>
       <c r="Q429">
-        <v>0.144844</v>
+        <v>0.14499000000000001</v>
       </c>
       <c r="R429">
-        <v>0.82078300000000004</v>
+        <v>0.82161200000000001</v>
       </c>
       <c r="S429">
-        <v>-11908.007766000001</v>
+        <v>-12447.400006</v>
       </c>
       <c r="T429">
-        <v>182303.86088600001</v>
+        <v>181275.39367600001</v>
       </c>
       <c r="U429">
-        <v>78928.644188000006</v>
+        <v>82355.667566999997</v>
       </c>
       <c r="V429">
-        <v>35.135880999999998</v>
+        <v>35.187023000000003</v>
       </c>
       <c r="W429">
-        <v>52.272295999999997</v>
+        <v>52.333621999999998</v>
       </c>
       <c r="X429">
-        <v>26.966768999999999</v>
+        <v>26.386915999999999</v>
       </c>
       <c r="Y429">
-        <v>17.653569000000001</v>
+        <v>18.19237</v>
       </c>
       <c r="Z429">
-        <v>36.372227000000002</v>
+        <v>37.713743999999998</v>
       </c>
       <c r="AA429">
-        <v>-9.9349999999999994E-2</v>
+        <v>-0.101368</v>
       </c>
     </row>
     <row r="430" spans="1:27" x14ac:dyDescent="0.35">
@@ -33922,13 +34080,13 @@
         <v>300</v>
       </c>
       <c r="B430">
-        <v>118000</v>
+        <v>122000</v>
       </c>
       <c r="C430">
         <v>900</v>
       </c>
       <c r="D430">
-        <v>118000</v>
+        <v>122000</v>
       </c>
       <c r="E430">
         <v>0.1</v>
@@ -33937,7 +34095,7 @@
         <v>300</v>
       </c>
       <c r="G430">
-        <v>5.8680999999999997E-2</v>
+        <v>5.7408000000000001E-2</v>
       </c>
       <c r="H430">
         <v>180</v>
@@ -33955,49 +34113,49 @@
         <v>40</v>
       </c>
       <c r="M430">
-        <v>35.003332999999998</v>
+        <v>34.998795999999999</v>
       </c>
       <c r="N430">
-        <v>89.743922999999995</v>
+        <v>89.731189999999998</v>
       </c>
       <c r="O430">
         <v>25</v>
       </c>
       <c r="P430">
-        <v>3.2733999999999999E-2</v>
+        <v>3.1747999999999998E-2</v>
       </c>
       <c r="Q430">
-        <v>0.14509</v>
+        <v>0.14523800000000001</v>
       </c>
       <c r="R430">
-        <v>0.82217600000000002</v>
+        <v>0.82301400000000002</v>
       </c>
       <c r="S430">
-        <v>-12617.879966</v>
+        <v>-13098.797603000001</v>
       </c>
       <c r="T430">
-        <v>180784.07061699999</v>
+        <v>179679.07263400001</v>
       </c>
       <c r="U430">
-        <v>84108.077862999999</v>
+        <v>87445.810874000003</v>
       </c>
       <c r="V430">
-        <v>35.219361999999997</v>
+        <v>35.271493999999997</v>
       </c>
       <c r="W430">
-        <v>52.374796000000003</v>
+        <v>52.437671000000002</v>
       </c>
       <c r="X430">
-        <v>26.033965999999999</v>
+        <v>25.437577000000001</v>
       </c>
       <c r="Y430">
-        <v>18.466432999999999</v>
+        <v>19.186050999999999</v>
       </c>
       <c r="Z430">
-        <v>38.476686000000001</v>
+        <v>40.219369</v>
       </c>
       <c r="AA430">
-        <v>-0.10433000000000001</v>
+        <v>-0.106861</v>
       </c>
     </row>
     <row r="431" spans="1:27" x14ac:dyDescent="0.35">
@@ -34005,13 +34163,13 @@
         <v>300</v>
       </c>
       <c r="B431">
-        <v>124000</v>
+        <v>128000</v>
       </c>
       <c r="C431">
         <v>900</v>
       </c>
       <c r="D431">
-        <v>124000</v>
+        <v>128000</v>
       </c>
       <c r="E431">
         <v>0.1</v>
@@ -34020,7 +34178,7 @@
         <v>300</v>
       </c>
       <c r="G431">
-        <v>5.6709000000000002E-2</v>
+        <v>5.5313000000000001E-2</v>
       </c>
       <c r="H431">
         <v>180</v>
@@ -34038,49 +34196,49 @@
         <v>40</v>
       </c>
       <c r="M431">
-        <v>35.004294000000002</v>
+        <v>35.003908000000003</v>
       </c>
       <c r="N431">
-        <v>89.725271000000006</v>
+        <v>89.713533999999996</v>
       </c>
       <c r="O431">
         <v>25</v>
       </c>
       <c r="P431">
-        <v>3.1140999999999999E-2</v>
+        <v>3.0012E-2</v>
       </c>
       <c r="Q431">
-        <v>0.14532900000000001</v>
+        <v>0.14549799999999999</v>
       </c>
       <c r="R431">
-        <v>0.82353100000000001</v>
+        <v>0.82448999999999995</v>
       </c>
       <c r="S431">
-        <v>-13315.611914999999</v>
+        <v>-13826.682252000001</v>
       </c>
       <c r="T431">
-        <v>179235.99956600001</v>
+        <v>178001.25260400001</v>
       </c>
       <c r="U431">
-        <v>89074.986067000005</v>
+        <v>92582.162356000001</v>
       </c>
       <c r="V431">
-        <v>35.301098000000003</v>
+        <v>35.358125000000001</v>
       </c>
       <c r="W431">
-        <v>52.475000000000001</v>
+        <v>52.546616</v>
       </c>
       <c r="X431">
-        <v>25.111314</v>
+        <v>24.460308000000001</v>
       </c>
       <c r="Y431">
-        <v>19.561799000000001</v>
+        <v>20.196408999999999</v>
       </c>
       <c r="Z431">
-        <v>41.197099999999999</v>
+        <v>42.862178999999998</v>
       </c>
       <c r="AA431">
-        <v>-0.108997</v>
+        <v>-0.11322</v>
       </c>
     </row>
     <row r="432" spans="1:27" x14ac:dyDescent="0.35">
@@ -34088,13 +34246,13 @@
         <v>300</v>
       </c>
       <c r="B432">
-        <v>130000</v>
+        <v>134000</v>
       </c>
       <c r="C432">
         <v>900</v>
       </c>
       <c r="D432">
-        <v>130000</v>
+        <v>134000</v>
       </c>
       <c r="E432">
         <v>0.1</v>
@@ -34103,7 +34261,7 @@
         <v>300</v>
       </c>
       <c r="G432">
-        <v>5.4658999999999999E-2</v>
+        <v>5.3310999999999997E-2</v>
       </c>
       <c r="H432">
         <v>180</v>
@@ -34121,49 +34279,49 @@
         <v>40</v>
       </c>
       <c r="M432">
-        <v>35.011808000000002</v>
+        <v>34.999561999999997</v>
       </c>
       <c r="N432">
-        <v>89.706756999999996</v>
+        <v>89.692618999999993</v>
       </c>
       <c r="O432">
         <v>25</v>
       </c>
       <c r="P432">
-        <v>2.947E-2</v>
+        <v>2.8372999999999999E-2</v>
       </c>
       <c r="Q432">
-        <v>0.14557999999999999</v>
+        <v>0.14574400000000001</v>
       </c>
       <c r="R432">
-        <v>0.82495099999999999</v>
+        <v>0.82588300000000003</v>
       </c>
       <c r="S432">
-        <v>-14086.680200000001</v>
+        <v>-14781.590063</v>
       </c>
       <c r="T432">
-        <v>177588.250788</v>
+        <v>176332.855106</v>
       </c>
       <c r="U432">
-        <v>93998.481899999999</v>
+        <v>97494.709363999995</v>
       </c>
       <c r="V432">
-        <v>35.384971999999998</v>
+        <v>35.440767999999998</v>
       </c>
       <c r="W432">
-        <v>52.58034</v>
+        <v>52.650767999999999</v>
       </c>
       <c r="X432">
-        <v>24.155463000000001</v>
+        <v>23.528144999999999</v>
       </c>
       <c r="Y432">
-        <v>20.427589000000001</v>
+        <v>20.988036999999998</v>
       </c>
       <c r="Z432">
-        <v>43.521917999999999</v>
+        <v>45.061836</v>
       </c>
       <c r="AA432">
-        <v>-0.114692</v>
+        <v>-0.11818099999999999</v>
       </c>
     </row>
     <row r="433" spans="1:27" x14ac:dyDescent="0.35">
@@ -34171,13 +34329,13 @@
         <v>300</v>
       </c>
       <c r="B433">
-        <v>136000</v>
+        <v>140000</v>
       </c>
       <c r="C433">
         <v>900</v>
       </c>
       <c r="D433">
-        <v>136000</v>
+        <v>140000</v>
       </c>
       <c r="E433">
         <v>0.1</v>
@@ -34186,7 +34344,7 @@
         <v>300</v>
       </c>
       <c r="G433">
-        <v>5.2588000000000003E-2</v>
+        <v>5.1187999999999997E-2</v>
       </c>
       <c r="H433">
         <v>180</v>
@@ -34204,49 +34362,49 @@
         <v>40</v>
       </c>
       <c r="M433">
-        <v>35.005333999999998</v>
+        <v>35.005674999999997</v>
       </c>
       <c r="N433">
-        <v>89.685985000000002</v>
+        <v>89.671104</v>
       </c>
       <c r="O433">
         <v>25</v>
       </c>
       <c r="P433">
-        <v>2.7720999999999999E-2</v>
+        <v>2.6516000000000001E-2</v>
       </c>
       <c r="Q433">
-        <v>0.145842</v>
+        <v>0.14602299999999999</v>
       </c>
       <c r="R433">
-        <v>0.82643699999999998</v>
+        <v>0.827461</v>
       </c>
       <c r="S433">
-        <v>-14997.928789</v>
+        <v>-15759.322920000001</v>
       </c>
       <c r="T433">
-        <v>175899.73058199999</v>
+        <v>174762.69146900001</v>
       </c>
       <c r="U433">
-        <v>99099.338361999995</v>
+        <v>102317.01027699999</v>
       </c>
       <c r="V433">
-        <v>35.472659</v>
+        <v>35.529696000000001</v>
       </c>
       <c r="W433">
-        <v>52.690753000000001</v>
+        <v>52.766776</v>
       </c>
       <c r="X433">
-        <v>23.192905</v>
+        <v>22.543614999999999</v>
       </c>
       <c r="Y433">
-        <v>21.439767</v>
+        <v>22.02233</v>
       </c>
       <c r="Z433">
-        <v>46.280520000000003</v>
+        <v>47.98901</v>
       </c>
       <c r="AA433">
-        <v>-0.12059499999999999</v>
+        <v>-0.124765</v>
       </c>
     </row>
     <row r="434" spans="1:27" x14ac:dyDescent="0.35">
@@ -34254,13 +34412,13 @@
         <v>300</v>
       </c>
       <c r="B434">
-        <v>142000</v>
+        <v>146000</v>
       </c>
       <c r="C434">
         <v>900</v>
       </c>
       <c r="D434">
-        <v>142000</v>
+        <v>146000</v>
       </c>
       <c r="E434">
         <v>0.1</v>
@@ -34269,7 +34427,7 @@
         <v>300</v>
       </c>
       <c r="G434">
-        <v>5.0465999999999997E-2</v>
+        <v>4.9196999999999998E-2</v>
       </c>
       <c r="H434">
         <v>180</v>
@@ -34287,49 +34445,49 @@
         <v>40</v>
       </c>
       <c r="M434">
-        <v>35.005856999999999</v>
+        <v>35.005569000000001</v>
       </c>
       <c r="N434">
-        <v>89.662267</v>
+        <v>89.643293999999997</v>
       </c>
       <c r="O434">
         <v>25</v>
       </c>
       <c r="P434">
-        <v>2.5884999999999998E-2</v>
+        <v>2.4763E-2</v>
       </c>
       <c r="Q434">
-        <v>0.146117</v>
+        <v>0.146285</v>
       </c>
       <c r="R434">
-        <v>0.82799699999999998</v>
+        <v>0.82895099999999999</v>
       </c>
       <c r="S434">
-        <v>-16130.381057000001</v>
+        <v>-16958.849021000002</v>
       </c>
       <c r="T434">
-        <v>174174.910619</v>
+        <v>173055.749515</v>
       </c>
       <c r="U434">
-        <v>103966.27854299999</v>
+        <v>106954.22412499999</v>
       </c>
       <c r="V434">
-        <v>35.561044000000003</v>
+        <v>35.616430000000001</v>
       </c>
       <c r="W434">
-        <v>52.806626000000001</v>
+        <v>52.877903000000003</v>
       </c>
       <c r="X434">
-        <v>22.209579000000002</v>
+        <v>21.623391000000002</v>
       </c>
       <c r="Y434">
-        <v>22.368662</v>
+        <v>23.019062999999999</v>
       </c>
       <c r="Z434">
-        <v>48.992921000000003</v>
+        <v>50.889370999999997</v>
       </c>
       <c r="AA434">
-        <v>-0.12714200000000001</v>
+        <v>-0.129356</v>
       </c>
     </row>
     <row r="435" spans="1:27" x14ac:dyDescent="0.35">
@@ -34337,13 +34495,13 @@
         <v>300</v>
       </c>
       <c r="B435">
-        <v>148000</v>
+        <v>152000</v>
       </c>
       <c r="C435">
         <v>900</v>
       </c>
       <c r="D435">
-        <v>148000</v>
+        <v>152000</v>
       </c>
       <c r="E435">
         <v>0.1</v>
@@ -34352,7 +34510,7 @@
         <v>300</v>
       </c>
       <c r="G435">
-        <v>4.8462999999999999E-2</v>
+        <v>4.7199999999999999E-2</v>
       </c>
       <c r="H435">
         <v>180</v>
@@ -34370,49 +34528,49 @@
         <v>40</v>
       </c>
       <c r="M435">
-        <v>35.006019999999999</v>
+        <v>35.006207000000003</v>
       </c>
       <c r="N435">
-        <v>89.630246</v>
+        <v>89.604134999999999</v>
       </c>
       <c r="O435">
         <v>25</v>
       </c>
       <c r="P435">
-        <v>2.4095999999999999E-2</v>
+        <v>2.2931E-2</v>
       </c>
       <c r="Q435">
-        <v>0.14638599999999999</v>
+        <v>0.14656</v>
       </c>
       <c r="R435">
-        <v>0.82951900000000001</v>
+        <v>0.83050900000000005</v>
       </c>
       <c r="S435">
-        <v>-17467.932581000001</v>
+        <v>-18678.742297000001</v>
       </c>
       <c r="T435">
-        <v>172497.42468600001</v>
+        <v>171450.44439300001</v>
       </c>
       <c r="U435">
-        <v>108521.866628</v>
+        <v>111309.157017</v>
       </c>
       <c r="V435">
-        <v>35.648904000000002</v>
+        <v>35.704649000000003</v>
       </c>
       <c r="W435">
-        <v>52.919736</v>
+        <v>52.993124000000002</v>
       </c>
       <c r="X435">
-        <v>21.284510999999998</v>
+        <v>20.702881000000001</v>
       </c>
       <c r="Y435">
-        <v>23.331762000000001</v>
+        <v>23.839053</v>
       </c>
       <c r="Z435">
-        <v>51.881171000000002</v>
+        <v>53.565373999999998</v>
       </c>
       <c r="AA435">
-        <v>-0.131883</v>
+        <v>-0.13395599999999999</v>
       </c>
     </row>
     <row r="436" spans="1:27" x14ac:dyDescent="0.35">
@@ -34420,13 +34578,13 @@
         <v>300</v>
       </c>
       <c r="B436">
-        <v>154000</v>
+        <v>158000</v>
       </c>
       <c r="C436">
         <v>900</v>
       </c>
       <c r="D436">
-        <v>154000</v>
+        <v>158000</v>
       </c>
       <c r="E436">
         <v>0.1</v>
@@ -34435,7 +34593,7 @@
         <v>300</v>
       </c>
       <c r="G436">
-        <v>4.6635000000000003E-2</v>
+        <v>4.5647E-2</v>
       </c>
       <c r="H436">
         <v>180</v>
@@ -34453,49 +34611,49 @@
         <v>40</v>
       </c>
       <c r="M436">
-        <v>35.006343999999999</v>
+        <v>35.005735999999999</v>
       </c>
       <c r="N436">
-        <v>89.586006999999995</v>
+        <v>89.547678000000005</v>
       </c>
       <c r="O436">
         <v>25</v>
       </c>
       <c r="P436">
-        <v>2.24E-2</v>
+        <v>2.1448999999999999E-2</v>
       </c>
       <c r="Q436">
-        <v>0.14663999999999999</v>
+        <v>0.146783</v>
       </c>
       <c r="R436">
-        <v>0.83096000000000003</v>
+        <v>0.83176799999999995</v>
       </c>
       <c r="S436">
-        <v>-19491.149169</v>
+        <v>-21114.598250999999</v>
       </c>
       <c r="T436">
-        <v>170992.32167400001</v>
+        <v>169840.09476400001</v>
       </c>
       <c r="U436">
-        <v>112548.990859</v>
+        <v>115056.419456</v>
       </c>
       <c r="V436">
-        <v>35.730065000000003</v>
+        <v>35.778426000000003</v>
       </c>
       <c r="W436">
-        <v>53.026528999999996</v>
+        <v>53.089320999999998</v>
       </c>
       <c r="X436">
-        <v>20.443394000000001</v>
+        <v>19.987590000000001</v>
       </c>
       <c r="Y436">
-        <v>24.042950999999999</v>
+        <v>24.589848</v>
       </c>
       <c r="Z436">
-        <v>54.290258000000001</v>
+        <v>56.031807000000001</v>
       </c>
       <c r="AA436">
-        <v>-0.134021</v>
+        <v>-0.13219400000000001</v>
       </c>
     </row>
     <row r="437" spans="1:27" x14ac:dyDescent="0.35">
@@ -34503,13 +34661,13 @@
         <v>300</v>
       </c>
       <c r="B437">
-        <v>160000</v>
+        <v>164000</v>
       </c>
       <c r="C437">
         <v>900</v>
       </c>
       <c r="D437">
-        <v>160000</v>
+        <v>164000</v>
       </c>
       <c r="E437">
         <v>0.1</v>
@@ -34518,7 +34676,7 @@
         <v>300</v>
       </c>
       <c r="G437">
-        <v>4.5435000000000003E-2</v>
+        <v>4.4420000000000001E-2</v>
       </c>
       <c r="H437">
         <v>180</v>
@@ -34536,49 +34694,49 @@
         <v>40</v>
       </c>
       <c r="M437">
-        <v>35.012653</v>
+        <v>35.005695000000003</v>
       </c>
       <c r="N437">
-        <v>89.529149000000004</v>
+        <v>89.479352000000006</v>
       </c>
       <c r="O437">
         <v>25</v>
       </c>
       <c r="P437">
-        <v>2.1222999999999999E-2</v>
+        <v>2.0244000000000002E-2</v>
       </c>
       <c r="Q437">
-        <v>0.146817</v>
+        <v>0.14696300000000001</v>
       </c>
       <c r="R437">
-        <v>0.83196000000000003</v>
+        <v>0.83279300000000001</v>
       </c>
       <c r="S437">
-        <v>-22102.156677999999</v>
+        <v>-24480.960605</v>
       </c>
       <c r="T437">
-        <v>169458.32500899999</v>
+        <v>168863.60239099999</v>
       </c>
       <c r="U437">
-        <v>115927.99632400001</v>
+        <v>117630.23684899999</v>
       </c>
       <c r="V437">
-        <v>35.788944000000001</v>
+        <v>35.829932999999997</v>
       </c>
       <c r="W437">
-        <v>53.104725999999999</v>
+        <v>53.164557000000002</v>
       </c>
       <c r="X437">
-        <v>19.890435</v>
+        <v>19.425388999999999</v>
       </c>
       <c r="Y437">
-        <v>24.670058000000001</v>
+        <v>25.184777</v>
       </c>
       <c r="Z437">
-        <v>56.352080999999998</v>
+        <v>58.081732000000002</v>
       </c>
       <c r="AA437">
-        <v>-0.12722700000000001</v>
+        <v>-0.12568599999999999</v>
       </c>
     </row>
     <row r="438" spans="1:27" x14ac:dyDescent="0.35">
@@ -34586,13 +34744,13 @@
         <v>300</v>
       </c>
       <c r="B438">
-        <v>166000</v>
+        <v>170000</v>
       </c>
       <c r="C438">
         <v>900</v>
       </c>
       <c r="D438">
-        <v>166000</v>
+        <v>170000</v>
       </c>
       <c r="E438">
         <v>0.1</v>
@@ -34601,7 +34759,7 @@
         <v>300</v>
       </c>
       <c r="G438">
-        <v>4.4239000000000001E-2</v>
+        <v>4.3526000000000002E-2</v>
       </c>
       <c r="H438">
         <v>180</v>
@@ -34619,49 +34777,49 @@
         <v>40</v>
       </c>
       <c r="M438">
-        <v>35.012810999999999</v>
+        <v>35.010824</v>
       </c>
       <c r="N438">
-        <v>89.452457999999993</v>
+        <v>89.387281999999999</v>
       </c>
       <c r="O438">
         <v>25</v>
       </c>
       <c r="P438">
-        <v>2.0036999999999999E-2</v>
+        <v>1.9328000000000001E-2</v>
       </c>
       <c r="Q438">
-        <v>0.14699400000000001</v>
+        <v>0.14710100000000001</v>
       </c>
       <c r="R438">
-        <v>0.83296800000000004</v>
+        <v>0.83357099999999995</v>
       </c>
       <c r="S438">
-        <v>-25671.731929000001</v>
+        <v>-28250.536368000001</v>
       </c>
       <c r="T438">
-        <v>168474.99811499999</v>
+        <v>167993.79947500001</v>
       </c>
       <c r="U438">
-        <v>118413.597567</v>
+        <v>119709.18354300001</v>
       </c>
       <c r="V438">
-        <v>35.841948000000002</v>
+        <v>35.873829000000001</v>
       </c>
       <c r="W438">
-        <v>53.17906</v>
+        <v>53.222512999999999</v>
       </c>
       <c r="X438">
-        <v>19.342476999999999</v>
+        <v>19.016860000000001</v>
       </c>
       <c r="Y438">
-        <v>25.293792</v>
+        <v>25.576989999999999</v>
       </c>
       <c r="Z438">
-        <v>58.472492000000003</v>
+        <v>59.559249999999999</v>
       </c>
       <c r="AA438">
-        <v>-0.120277</v>
+        <v>-0.114414</v>
       </c>
     </row>
     <row r="439" spans="1:27" x14ac:dyDescent="0.35">
@@ -34669,13 +34827,13 @@
         <v>300</v>
       </c>
       <c r="B439">
-        <v>172000</v>
+        <v>176000</v>
       </c>
       <c r="C439">
         <v>900</v>
       </c>
       <c r="D439">
-        <v>172000</v>
+        <v>176000</v>
       </c>
       <c r="E439">
         <v>0.1</v>
@@ -34684,7 +34842,7 @@
         <v>300</v>
       </c>
       <c r="G439">
-        <v>4.3343E-2</v>
+        <v>4.2812999999999997E-2</v>
       </c>
       <c r="H439">
         <v>180</v>
@@ -34702,49 +34860,49 @@
         <v>40</v>
       </c>
       <c r="M439">
-        <v>35.011139</v>
+        <v>35.003272000000003</v>
       </c>
       <c r="N439">
-        <v>89.353790000000004</v>
+        <v>89.285200000000003</v>
       </c>
       <c r="O439">
         <v>25</v>
       </c>
       <c r="P439">
-        <v>1.9103999999999999E-2</v>
+        <v>1.8565000000000002E-2</v>
       </c>
       <c r="Q439">
-        <v>0.14713399999999999</v>
+        <v>0.14721500000000001</v>
       </c>
       <c r="R439">
-        <v>0.833762</v>
+        <v>0.83421900000000004</v>
       </c>
       <c r="S439">
-        <v>-29727.212702000001</v>
+        <v>-32712.448779999999</v>
       </c>
       <c r="T439">
-        <v>168590.542556</v>
+        <v>168082.32678900001</v>
       </c>
       <c r="U439">
-        <v>119462.85419699999</v>
+        <v>120669.80497300001</v>
       </c>
       <c r="V439">
-        <v>35.88008</v>
+        <v>35.907778999999998</v>
       </c>
       <c r="W439">
-        <v>53.231655000000003</v>
+        <v>53.265464000000001</v>
       </c>
       <c r="X439">
-        <v>18.932434000000001</v>
+        <v>18.690852</v>
       </c>
       <c r="Y439">
-        <v>25.702645</v>
+        <v>25.843855000000001</v>
       </c>
       <c r="Z439">
-        <v>60.017308999999997</v>
+        <v>60.694017000000002</v>
       </c>
       <c r="AA439">
-        <v>-0.109052</v>
+        <v>-0.10058400000000001</v>
       </c>
     </row>
     <row r="440" spans="1:27" x14ac:dyDescent="0.35">
@@ -34752,13 +34910,13 @@
         <v>300</v>
       </c>
       <c r="B440">
-        <v>178000</v>
+        <v>182000</v>
       </c>
       <c r="C440">
         <v>900</v>
       </c>
       <c r="D440">
-        <v>178000</v>
+        <v>182000</v>
       </c>
       <c r="E440">
         <v>0.1</v>
@@ -34767,7 +34925,7 @@
         <v>300</v>
       </c>
       <c r="G440">
-        <v>4.2432999999999998E-2</v>
+        <v>4.2116000000000001E-2</v>
       </c>
       <c r="H440">
         <v>180</v>
@@ -34785,49 +34943,49 @@
         <v>40</v>
       </c>
       <c r="M440">
-        <v>35.005363000000003</v>
+        <v>35.009410000000003</v>
       </c>
       <c r="N440">
-        <v>89.246815999999995</v>
+        <v>89.182827000000003</v>
       </c>
       <c r="O440">
         <v>25</v>
       </c>
       <c r="P440">
-        <v>1.8207999999999998E-2</v>
+        <v>1.7868999999999999E-2</v>
       </c>
       <c r="Q440">
-        <v>0.14726900000000001</v>
+        <v>0.14732000000000001</v>
       </c>
       <c r="R440">
-        <v>0.83452300000000001</v>
+        <v>0.83481099999999997</v>
       </c>
       <c r="S440">
-        <v>-34209.724555000001</v>
+        <v>-37415.353174000003</v>
       </c>
       <c r="T440">
-        <v>167264.48859299999</v>
+        <v>166913.26383000001</v>
       </c>
       <c r="U440">
-        <v>121875.83519100001</v>
+        <v>122659.52912799999</v>
       </c>
       <c r="V440">
-        <v>35.931438</v>
+        <v>35.942314000000003</v>
       </c>
       <c r="W440">
-        <v>53.291227999999997</v>
+        <v>53.312824999999997</v>
       </c>
       <c r="X440">
-        <v>18.517415</v>
+        <v>18.372899</v>
       </c>
       <c r="Y440">
-        <v>25.970123999999998</v>
+        <v>26.16112</v>
       </c>
       <c r="Z440">
-        <v>61.204053000000002</v>
+        <v>61.891889999999997</v>
       </c>
       <c r="AA440">
-        <v>-9.7982E-2</v>
+        <v>-8.6503999999999998E-2</v>
       </c>
     </row>
     <row r="441" spans="1:27" x14ac:dyDescent="0.35">
@@ -34835,13 +34993,13 @@
         <v>300</v>
       </c>
       <c r="B441">
-        <v>184000</v>
+        <v>188000</v>
       </c>
       <c r="C441">
         <v>900</v>
       </c>
       <c r="D441">
-        <v>184000</v>
+        <v>188000</v>
       </c>
       <c r="E441">
         <v>0.1</v>
@@ -34850,7 +35008,7 @@
         <v>300</v>
       </c>
       <c r="G441">
-        <v>4.1971000000000001E-2</v>
+        <v>4.163E-2</v>
       </c>
       <c r="H441">
         <v>180</v>
@@ -34868,49 +35026,49 @@
         <v>40</v>
       </c>
       <c r="M441">
-        <v>35.003872999999999</v>
+        <v>35.008544000000001</v>
       </c>
       <c r="N441">
-        <v>89.151017999999993</v>
+        <v>89.080467999999996</v>
       </c>
       <c r="O441">
         <v>25</v>
       </c>
       <c r="P441">
-        <v>1.7680999999999999E-2</v>
+        <v>1.7333000000000001E-2</v>
       </c>
       <c r="Q441">
-        <v>0.14734800000000001</v>
+        <v>0.1474</v>
       </c>
       <c r="R441">
-        <v>0.83497100000000002</v>
+        <v>0.83526699999999998</v>
       </c>
       <c r="S441">
-        <v>-38919.996361999998</v>
+        <v>-42417.651483000001</v>
       </c>
       <c r="T441">
-        <v>167323.927582</v>
+        <v>166976.280742</v>
       </c>
       <c r="U441">
-        <v>122481.03260999999</v>
+        <v>123237.45033000001</v>
       </c>
       <c r="V441">
-        <v>35.947600000000001</v>
+        <v>35.959860999999997</v>
       </c>
       <c r="W441">
-        <v>53.320855000000002</v>
+        <v>53.342871000000002</v>
       </c>
       <c r="X441">
-        <v>18.306832</v>
+        <v>18.15194</v>
       </c>
       <c r="Y441">
-        <v>26.251404000000001</v>
+        <v>26.461532999999999</v>
       </c>
       <c r="Z441">
-        <v>62.258833000000003</v>
+        <v>62.996679999999998</v>
       </c>
       <c r="AA441">
-        <v>-8.0574000000000007E-2</v>
+        <v>-6.9417999999999994E-2</v>
       </c>
     </row>
     <row r="442" spans="1:27" x14ac:dyDescent="0.35">
@@ -34918,13 +35076,13 @@
         <v>300</v>
       </c>
       <c r="B442">
-        <v>190000</v>
+        <v>194000</v>
       </c>
       <c r="C442">
         <v>900</v>
       </c>
       <c r="D442">
-        <v>190000</v>
+        <v>194000</v>
       </c>
       <c r="E442">
         <v>0.1</v>
@@ -34933,7 +35091,7 @@
         <v>300</v>
       </c>
       <c r="G442">
-        <v>4.1279000000000003E-2</v>
+        <v>4.1075E-2</v>
       </c>
       <c r="H442">
         <v>180</v>
@@ -34951,49 +35109,49 @@
         <v>40</v>
       </c>
       <c r="M442">
-        <v>35.006011000000001</v>
+        <v>35.008637999999998</v>
       </c>
       <c r="N442">
-        <v>89.034893999999994</v>
+        <v>88.981603000000007</v>
       </c>
       <c r="O442">
         <v>25</v>
       </c>
       <c r="P442">
-        <v>1.6972999999999999E-2</v>
+        <v>1.6750000000000001E-2</v>
       </c>
       <c r="Q442">
-        <v>0.147454</v>
+        <v>0.14748700000000001</v>
       </c>
       <c r="R442">
-        <v>0.83557300000000001</v>
+        <v>0.835762</v>
       </c>
       <c r="S442">
-        <v>-43860.807692000002</v>
+        <v>-46575.173433999997</v>
       </c>
       <c r="T442">
-        <v>166412.56161599999</v>
+        <v>166105.08896299999</v>
       </c>
       <c r="U442">
-        <v>124153.28945</v>
+        <v>124752.112165</v>
       </c>
       <c r="V442">
-        <v>35.987672000000003</v>
+        <v>35.995018000000002</v>
       </c>
       <c r="W442">
-        <v>53.367171999999997</v>
+        <v>53.381895</v>
       </c>
       <c r="X442">
-        <v>17.991617000000002</v>
+        <v>17.898885</v>
       </c>
       <c r="Y442">
-        <v>26.533007000000001</v>
+        <v>26.618589</v>
       </c>
       <c r="Z442">
-        <v>63.414551000000003</v>
+        <v>63.785749000000003</v>
       </c>
       <c r="AA442">
-        <v>-6.6408999999999996E-2</v>
+        <v>-5.3325999999999998E-2</v>
       </c>
     </row>
     <row r="443" spans="1:27" x14ac:dyDescent="0.35">
@@ -35001,13 +35159,13 @@
         <v>300</v>
       </c>
       <c r="B443">
-        <v>196000</v>
+        <v>200000</v>
       </c>
       <c r="C443">
         <v>900</v>
       </c>
       <c r="D443">
-        <v>196000</v>
+        <v>200000</v>
       </c>
       <c r="E443">
         <v>0.1</v>
@@ -35016,7 +35174,7 @@
         <v>300</v>
       </c>
       <c r="G443">
-        <v>4.0891999999999998E-2</v>
+        <v>4.0624E-2</v>
       </c>
       <c r="H443">
         <v>180</v>
@@ -35034,49 +35192,49 @@
         <v>40</v>
       </c>
       <c r="M443">
-        <v>35.005673000000002</v>
+        <v>35.005631000000001</v>
       </c>
       <c r="N443">
-        <v>88.924318999999997</v>
+        <v>88.848733999999993</v>
       </c>
       <c r="O443">
         <v>25</v>
       </c>
       <c r="P443">
-        <v>1.6518999999999999E-2</v>
+        <v>1.6233000000000001E-2</v>
       </c>
       <c r="Q443">
-        <v>0.14752199999999999</v>
+        <v>0.147565</v>
       </c>
       <c r="R443">
-        <v>0.83595799999999998</v>
+        <v>0.836202</v>
       </c>
       <c r="S443">
-        <v>-48931.393834000002</v>
+        <v>-52528.384311000002</v>
       </c>
       <c r="T443">
-        <v>166463.019004</v>
+        <v>166162.87314000001</v>
       </c>
       <c r="U443">
-        <v>124648.053764</v>
+        <v>125272.84035</v>
       </c>
       <c r="V443">
-        <v>36.006098999999999</v>
+        <v>36.019058000000001</v>
       </c>
       <c r="W443">
-        <v>53.392558000000001</v>
+        <v>53.410839000000003</v>
       </c>
       <c r="X443">
-        <v>17.815611000000001</v>
+        <v>17.694091</v>
       </c>
       <c r="Y443">
-        <v>26.727847000000001</v>
+        <v>26.855155</v>
       </c>
       <c r="Z443">
-        <v>64.240915000000001</v>
+        <v>64.762728999999993</v>
       </c>
       <c r="AA443">
-        <v>-4.7928999999999999E-2</v>
+        <v>-3.5739E-2</v>
       </c>
     </row>
   </sheetData>
@@ -35097,9 +35255,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -35312,27 +35473,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A6ED6D0-FE53-4BFC-8DEF-82D0D9F0E993}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2B5FC1-AD94-452E-B48E-8A2F9B1C8C34}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="95507c7c-a837-40bb-8a3d-470d6a1609d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -35357,9 +35506,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2B5FC1-AD94-452E-B48E-8A2F9B1C8C34}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A6ED6D0-FE53-4BFC-8DEF-82D0D9F0E993}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="95507c7c-a837-40bb-8a3d-470d6a1609d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated fast run results with reruns
</commit_message>
<xml_diff>
--- a/fast run results.xlsx
+++ b/fast run results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - Imperial College London\School Work\Year 4\Research project\GITTO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3774\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="114_{5B84B35A-4784-4095-8A35-73569DC69E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B0B3559A-7F38-4F5D-B096-DE29307C09B3}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="114_{5B84B35A-4784-4095-8A35-73569DC69E44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E2A26A32-0EEF-4FDE-BF43-56CBC3B097B3}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>Inputs - Sour gas flowrate</t>
   </si>
@@ -175,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -183,6 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,18 +501,18 @@
   <dimension ref="A1:AA443"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Q411" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Q123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S417" sqref="S417"/>
+      <selection pane="bottomRight" activeCell="W138" sqref="W138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="27" width="12.6328125" customWidth="1"/>
+    <col min="1" max="27" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="47.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +595,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -659,7 +660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>40</v>
       </c>
@@ -742,7 +743,7 @@
         <v>0.146145</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40</v>
       </c>
@@ -825,7 +826,7 @@
         <v>0.17005999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -908,7 +909,7 @@
         <v>0.19358</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40</v>
       </c>
@@ -991,7 +992,7 @@
         <v>0.21715599999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>40</v>
       </c>
@@ -1074,7 +1075,7 @@
         <v>0.240874</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>40</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>0.26455400000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>40</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>0.288323</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>0.31208900000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>40</v>
       </c>
@@ -1406,7 +1407,7 @@
         <v>0.33588200000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>40</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>0.35969099999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>40</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>0.38354199999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>40</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>0.40738099999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>40</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>0.43122300000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>40</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>0.45505800000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>40</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>0.47888199999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>40</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>0.50274399999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>40</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>0.52660799999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>40</v>
       </c>
@@ -2153,7 +2154,7 @@
         <v>0.55048200000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>40</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>0.57434399999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>40</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>0.59822699999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>40</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>0.62211000000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>53</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>9.6296999999999994E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>53</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>0.119646</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>53</v>
       </c>
@@ -2651,7 +2652,7 @@
         <v>0.14286399999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>53</v>
       </c>
@@ -2734,7 +2735,7 @@
         <v>0.16617299999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>53</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>0.19012599999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>53</v>
       </c>
@@ -2900,7 +2901,7 @@
         <v>0.21380199999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>53</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>0.23766000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>53</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>0.261019</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>53</v>
       </c>
@@ -3149,7 +3150,7 @@
         <v>0.28495199999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>53</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>0.30788500000000002</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>53</v>
       </c>
@@ -3315,7 +3316,7 @@
         <v>0.33182200000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>53</v>
       </c>
@@ -3398,7 +3399,7 @@
         <v>0.35553600000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>53</v>
       </c>
@@ -3481,7 +3482,7 @@
         <v>0.37926599999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>53</v>
       </c>
@@ -3564,7 +3565,7 @@
         <v>0.40302900000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>53</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>0.42683399999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>53</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>0.45060299999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>0.47440199999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>53</v>
       </c>
@@ -3896,7 +3897,7 @@
         <v>0.49798799999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>53</v>
       </c>
@@ -3979,7 +3980,7 @@
         <v>0.52200000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>53</v>
       </c>
@@ -4062,7 +4063,7 @@
         <v>0.54574699999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>53</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>0.56955100000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>66</v>
       </c>
@@ -4228,7 +4229,7 @@
         <v>5.2988E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>66</v>
       </c>
@@ -4311,7 +4312,7 @@
         <v>7.3391999999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>66</v>
       </c>
@@ -4394,7 +4395,7 @@
         <v>9.6324000000000007E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>66</v>
       </c>
@@ -4477,7 +4478,7 @@
         <v>0.11952400000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>66</v>
       </c>
@@ -4560,7 +4561,7 @@
         <v>0.14183999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>66</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>0.16634599999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>66</v>
       </c>
@@ -4726,7 +4727,7 @@
         <v>0.18958700000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>66</v>
       </c>
@@ -4809,7 +4810,7 @@
         <v>0.21216399999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>66</v>
       </c>
@@ -4892,7 +4893,7 @@
         <v>0.23597899999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>66</v>
       </c>
@@ -4975,7 +4976,7 @@
         <v>0.25989200000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>66</v>
       </c>
@@ -5058,7 +5059,7 @@
         <v>0.28282400000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>66</v>
       </c>
@@ -5141,7 +5142,7 @@
         <v>0.30692399999999997</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>66</v>
       </c>
@@ -5224,7 +5225,7 @@
         <v>0.33054800000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>66</v>
       </c>
@@ -5307,7 +5308,7 @@
         <v>0.35393400000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>66</v>
       </c>
@@ -5390,7 +5391,7 @@
         <v>0.377641</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>66</v>
       </c>
@@ -5473,7 +5474,7 @@
         <v>0.40121899999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>66</v>
       </c>
@@ -5556,7 +5557,7 @@
         <v>0.42496800000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>66</v>
       </c>
@@ -5639,7 +5640,7 @@
         <v>0.44868599999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>66</v>
       </c>
@@ -5722,7 +5723,7 @@
         <v>0.47231800000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>66</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>0.49609999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>66</v>
       </c>
@@ -5888,7 +5889,7 @@
         <v>0.51938799999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>79</v>
       </c>
@@ -5971,7 +5972,7 @@
         <v>1.1091999999999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>79</v>
       </c>
@@ -6054,7 +6055,7 @@
         <v>3.2091000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>79</v>
       </c>
@@ -6137,7 +6138,7 @@
         <v>5.2881999999999998E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>79</v>
       </c>
@@ -6220,7 +6221,7 @@
         <v>7.7229000000000006E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>79</v>
       </c>
@@ -6303,7 +6304,7 @@
         <v>9.8289000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>79</v>
       </c>
@@ -6386,7 +6387,7 @@
         <v>0.121571</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>79</v>
       </c>
@@ -6469,7 +6470,7 @@
         <v>0.144786</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>79</v>
       </c>
@@ -6552,7 +6553,7 @@
         <v>0.16638500000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>79</v>
       </c>
@@ -6635,7 +6636,7 @@
         <v>0.19064300000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>79</v>
       </c>
@@ -6718,7 +6719,7 @@
         <v>0.21352499999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>79</v>
       </c>
@@ -6801,7 +6802,7 @@
         <v>0.23672899999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>79</v>
       </c>
@@ -6884,7 +6885,7 @@
         <v>0.26002599999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>79</v>
       </c>
@@ -6967,7 +6968,7 @@
         <v>0.28378900000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>79</v>
       </c>
@@ -7050,7 +7051,7 @@
         <v>0.30682799999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7133,7 +7134,7 @@
         <v>0.33085999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -7216,7 +7217,7 @@
         <v>0.35423100000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
@@ -7299,7 +7300,7 @@
         <v>0.37786999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>79</v>
       </c>
@@ -7382,7 +7383,7 @@
         <v>0.40099400000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>79</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>0.42503800000000003</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>79</v>
       </c>
@@ -7548,7 +7549,7 @@
         <v>0.44864700000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>79</v>
       </c>
@@ -7631,7 +7632,7 @@
         <v>0.47233399999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>92</v>
       </c>
@@ -7714,7 +7715,7 @@
         <v>-2.3945999999999999E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>92</v>
       </c>
@@ -7797,7 +7798,7 @@
         <v>-8.9119999999999998E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>92</v>
       </c>
@@ -7880,7 +7881,7 @@
         <v>1.5079E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>92</v>
       </c>
@@ -7963,7 +7964,7 @@
         <v>3.5871E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>92</v>
       </c>
@@ -8046,7 +8047,7 @@
         <v>5.5973000000000002E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>92</v>
       </c>
@@ -8129,7 +8130,7 @@
         <v>7.9069E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8212,7 +8213,7 @@
         <v>0.102715</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -8295,7 +8296,7 @@
         <v>0.12485300000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>92</v>
       </c>
@@ -8378,7 +8379,7 @@
         <v>0.14695800000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>92</v>
       </c>
@@ -8461,7 +8462,7 @@
         <v>0.17035800000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>92</v>
       </c>
@@ -8544,18 +8545,18 @@
         <v>0.19373599999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A98">
+    <row r="98" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
         <v>92</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="4">
         <v>146000</v>
       </c>
       <c r="C98">
         <v>276</v>
       </c>
       <c r="D98">
-        <v>140000</v>
+        <v>146000</v>
       </c>
       <c r="E98">
         <v>0.1</v>
@@ -8563,8 +8564,8 @@
       <c r="F98">
         <v>92</v>
       </c>
-      <c r="G98">
-        <v>1.4638999999999999E-2</v>
+      <c r="G98" s="5">
+        <v>1.4295212817667401E-2</v>
       </c>
       <c r="H98">
         <v>180</v>
@@ -8582,52 +8583,52 @@
         <v>40</v>
       </c>
       <c r="M98">
-        <v>35.002338999999999</v>
+        <v>35.007065821383399</v>
       </c>
       <c r="N98">
-        <v>84.364401000000001</v>
+        <v>84.048318582309307</v>
       </c>
       <c r="O98">
         <v>25</v>
       </c>
-      <c r="P98">
-        <v>8.2120000000000005E-3</v>
+      <c r="P98" s="5">
+        <v>7.8212613236464494E-3</v>
       </c>
       <c r="Q98">
-        <v>0.14876800000000001</v>
+        <v>0.14882681080145299</v>
       </c>
       <c r="R98">
-        <v>0.84301999999999999</v>
+        <v>0.84335192787490099</v>
       </c>
       <c r="S98">
-        <v>-86145.427291999993</v>
+        <v>-92251.597837909998</v>
       </c>
       <c r="T98">
-        <v>45185.027056999999</v>
+        <v>45124.8228818426</v>
       </c>
       <c r="U98">
-        <v>46539.996437000002</v>
+        <v>46598.177902857497</v>
       </c>
       <c r="V98">
-        <v>11.182406</v>
+        <v>11.1771901103112</v>
       </c>
       <c r="W98">
-        <v>16.550017</v>
+        <v>16.5577890969859</v>
       </c>
       <c r="X98">
-        <v>1.905732</v>
+        <v>1.8600667724037101</v>
       </c>
       <c r="Y98">
-        <v>11.745513000000001</v>
+        <v>11.800443371837799</v>
       </c>
       <c r="Z98">
-        <v>83.594402000000002</v>
+        <v>84.610363435340304</v>
       </c>
       <c r="AA98">
-        <v>0.19373599999999999</v>
-      </c>
-    </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
+        <v>0.216256263437859</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>92</v>
       </c>
@@ -8710,7 +8711,7 @@
         <v>0.239228</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>92</v>
       </c>
@@ -8793,7 +8794,7 @@
         <v>0.26292900000000002</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>92</v>
       </c>
@@ -8876,7 +8877,7 @@
         <v>0.28614600000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>92</v>
       </c>
@@ -8959,7 +8960,7 @@
         <v>0.30944500000000003</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>92</v>
       </c>
@@ -9042,7 +9043,7 @@
         <v>0.33282899999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>92</v>
       </c>
@@ -9125,7 +9126,7 @@
         <v>0.35662899999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>92</v>
       </c>
@@ -9208,7 +9209,7 @@
         <v>0.38000800000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>92</v>
       </c>
@@ -9291,7 +9292,7 @@
         <v>0.40354200000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>92</v>
       </c>
@@ -9374,7 +9375,7 @@
         <v>0.42713699999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105</v>
       </c>
@@ -9457,7 +9458,7 @@
         <v>-5.1768000000000002E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>105</v>
       </c>
@@ -9540,7 +9541,7 @@
         <v>-4.3607E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>105</v>
       </c>
@@ -9623,7 +9624,7 @@
         <v>-2.0947E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>105</v>
       </c>
@@ -9706,7 +9707,7 @@
         <v>-2.4009999999999999E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>105</v>
       </c>
@@ -9789,7 +9790,7 @@
         <v>1.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>105</v>
       </c>
@@ -9872,7 +9873,7 @@
         <v>4.1658000000000001E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>105</v>
       </c>
@@ -9955,7 +9956,7 @@
         <v>6.5784999999999996E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>105</v>
       </c>
@@ -10038,7 +10039,7 @@
         <v>8.4265999999999994E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>105</v>
       </c>
@@ -10121,7 +10122,7 @@
         <v>0.108629</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>105</v>
       </c>
@@ -10204,7 +10205,7 @@
         <v>0.12955800000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>105</v>
       </c>
@@ -10287,7 +10288,7 @@
         <v>0.15218699999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>105</v>
       </c>
@@ -10370,7 +10371,7 @@
         <v>0.17498</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>105</v>
       </c>
@@ -10453,7 +10454,7 @@
         <v>0.19881599999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>105</v>
       </c>
@@ -10536,7 +10537,7 @@
         <v>0.221696</v>
       </c>
     </row>
-    <row r="122" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>105</v>
       </c>
@@ -10619,7 +10620,7 @@
         <v>0.24440500000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>105</v>
       </c>
@@ -10702,7 +10703,7 @@
         <v>0.26766200000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>105</v>
       </c>
@@ -10785,7 +10786,7 @@
         <v>0.29054799999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>105</v>
       </c>
@@ -10868,7 +10869,7 @@
         <v>0.31373200000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>105</v>
       </c>
@@ -10951,7 +10952,7 @@
         <v>0.33741900000000002</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>105</v>
       </c>
@@ -11034,7 +11035,7 @@
         <v>0.36032900000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>105</v>
       </c>
@@ -11117,7 +11118,7 @@
         <v>0.38419399999999998</v>
       </c>
     </row>
-    <row r="129" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>118</v>
       </c>
@@ -11125,7 +11126,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>118</v>
       </c>
@@ -11208,7 +11209,7 @@
         <v>-6.3297000000000006E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>118</v>
       </c>
@@ -11291,7 +11292,7 @@
         <v>-5.0113999999999999E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>118</v>
       </c>
@@ -11374,7 +11375,7 @@
         <v>-3.5173000000000003E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>118</v>
       </c>
@@ -11457,18 +11458,18 @@
         <v>-1.3795E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A134">
+    <row r="134" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4">
         <v>118</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="4">
         <v>110000</v>
       </c>
       <c r="C134">
         <v>354</v>
       </c>
       <c r="D134">
-        <v>104000</v>
+        <v>110000</v>
       </c>
       <c r="E134">
         <v>0.1</v>
@@ -11476,8 +11477,8 @@
       <c r="F134">
         <v>118</v>
       </c>
-      <c r="G134">
-        <v>2.2012E-2</v>
+      <c r="G134" s="5">
+        <v>2.1336787908721899E-2</v>
       </c>
       <c r="H134">
         <v>180</v>
@@ -11495,52 +11496,52 @@
         <v>40</v>
       </c>
       <c r="M134">
-        <v>34.998685999999999</v>
+        <v>35.002061755422197</v>
       </c>
       <c r="N134">
-        <v>87.880009000000001</v>
+        <v>87.602130768646006</v>
       </c>
       <c r="O134">
         <v>25</v>
       </c>
-      <c r="P134">
-        <v>1.2886E-2</v>
+      <c r="P134" s="5">
+        <v>1.2251057749997799E-2</v>
       </c>
       <c r="Q134">
-        <v>0.148067</v>
+        <v>0.1481623413375</v>
       </c>
       <c r="R134">
-        <v>0.83904699999999999</v>
+        <v>0.83958660091250203</v>
       </c>
       <c r="S134">
-        <v>-38899.904978999999</v>
+        <v>-44584.702784960202</v>
       </c>
       <c r="T134">
-        <v>60448.899642999997</v>
+        <v>60186.926749234597</v>
       </c>
       <c r="U134">
-        <v>55545.507638000003</v>
+        <v>55984.019705653896</v>
       </c>
       <c r="V134">
-        <v>14.243408000000001</v>
+        <v>14.2498101312468</v>
       </c>
       <c r="W134">
-        <v>21.098846999999999</v>
+        <v>21.116144468526102</v>
       </c>
       <c r="X134">
-        <v>3.708021</v>
+        <v>3.5910038920638199</v>
       </c>
       <c r="Y134">
-        <v>13.844402000000001</v>
+        <v>13.924220577597</v>
       </c>
       <c r="Z134">
-        <v>74.629240999999993</v>
-      </c>
-      <c r="AA134">
-        <v>-1.3795E-2</v>
-      </c>
-    </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.35">
+        <v>76.234948069192399</v>
+      </c>
+      <c r="AA134" s="5">
+        <v>6.5138581919266803E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>118</v>
       </c>
@@ -11623,7 +11624,7 @@
         <v>2.7241999999999999E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>118</v>
       </c>
@@ -11706,7 +11707,7 @@
         <v>4.8718999999999998E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>118</v>
       </c>
@@ -11789,7 +11790,7 @@
         <v>7.1651000000000006E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>118</v>
       </c>
@@ -11872,7 +11873,7 @@
         <v>9.1467000000000007E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>118</v>
       </c>
@@ -11955,7 +11956,7 @@
         <v>0.11525100000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>118</v>
       </c>
@@ -12038,7 +12039,7 @@
         <v>0.137099</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>118</v>
       </c>
@@ -12121,7 +12122,7 @@
         <v>0.15978400000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>118</v>
       </c>
@@ -12204,7 +12205,7 @@
         <v>0.18288199999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>118</v>
       </c>
@@ -12287,7 +12288,7 @@
         <v>0.205677</v>
       </c>
     </row>
-    <row r="144" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>118</v>
       </c>
@@ -12370,7 +12371,7 @@
         <v>0.227851</v>
       </c>
     </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>118</v>
       </c>
@@ -12453,7 +12454,7 @@
         <v>0.25126900000000002</v>
       </c>
     </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>118</v>
       </c>
@@ -12536,7 +12537,7 @@
         <v>0.27424199999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>118</v>
       </c>
@@ -12619,7 +12620,7 @@
         <v>0.297375</v>
       </c>
     </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>118</v>
       </c>
@@ -12702,7 +12703,7 @@
         <v>0.320104</v>
       </c>
     </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>118</v>
       </c>
@@ -12785,7 +12786,7 @@
         <v>0.343308</v>
       </c>
     </row>
-    <row r="150" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>131</v>
       </c>
@@ -12793,7 +12794,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>131</v>
       </c>
@@ -12876,7 +12877,7 @@
         <v>-9.8936999999999997E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>131</v>
       </c>
@@ -12959,7 +12960,7 @@
         <v>-8.2562999999999998E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>131</v>
       </c>
@@ -13042,7 +13043,7 @@
         <v>-6.4979999999999996E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>131</v>
       </c>
@@ -13125,7 +13126,7 @@
         <v>-4.6594999999999998E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>131</v>
       </c>
@@ -13208,7 +13209,7 @@
         <v>-2.8187E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>131</v>
       </c>
@@ -13291,7 +13292,7 @@
         <v>-5.914E-3</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>131</v>
       </c>
@@ -13374,7 +13375,7 @@
         <v>1.4344000000000001E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>131</v>
       </c>
@@ -13457,7 +13458,7 @@
         <v>3.5298000000000003E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>131</v>
       </c>
@@ -13540,7 +13541,7 @@
         <v>5.7890999999999998E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>131</v>
       </c>
@@ -13623,7 +13624,7 @@
         <v>7.9713999999999993E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>131</v>
       </c>
@@ -13706,7 +13707,7 @@
         <v>0.101572</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>131</v>
       </c>
@@ -13789,7 +13790,7 @@
         <v>0.123608</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>131</v>
       </c>
@@ -13872,7 +13873,7 @@
         <v>0.14586099999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>131</v>
       </c>
@@ -13955,7 +13956,7 @@
         <v>0.168573</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>131</v>
       </c>
@@ -14038,7 +14039,7 @@
         <v>0.19050700000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>131</v>
       </c>
@@ -14121,7 +14122,7 @@
         <v>0.21306700000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>131</v>
       </c>
@@ -14204,7 +14205,7 @@
         <v>0.23574999999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>131</v>
       </c>
@@ -14287,7 +14288,7 @@
         <v>0.25929400000000002</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>131</v>
       </c>
@@ -14370,7 +14371,7 @@
         <v>0.28209699999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>131</v>
       </c>
@@ -14453,7 +14454,7 @@
         <v>0.30505500000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>144</v>
       </c>
@@ -14461,7 +14462,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>144</v>
       </c>
@@ -14544,7 +14545,7 @@
         <v>-0.11629</v>
       </c>
     </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>144</v>
       </c>
@@ -14627,7 +14628,7 @@
         <v>-0.104916</v>
       </c>
     </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>144</v>
       </c>
@@ -14710,7 +14711,7 @@
         <v>-9.0886999999999996E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>144</v>
       </c>
@@ -14793,7 +14794,7 @@
         <v>-7.3395000000000002E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>144</v>
       </c>
@@ -14876,7 +14877,7 @@
         <v>-5.6264000000000002E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>144</v>
       </c>
@@ -14959,7 +14960,7 @@
         <v>-3.5902000000000003E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>144</v>
       </c>
@@ -15042,7 +15043,7 @@
         <v>-1.5786000000000001E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>144</v>
       </c>
@@ -15125,7 +15126,7 @@
         <v>3.3110000000000001E-3</v>
       </c>
     </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>144</v>
       </c>
@@ -15208,7 +15209,7 @@
         <v>2.5610000000000001E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>144</v>
       </c>
@@ -15291,7 +15292,7 @@
         <v>4.632E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>144</v>
       </c>
@@ -15374,7 +15375,7 @@
         <v>6.7734000000000003E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>144</v>
       </c>
@@ -15457,7 +15458,7 @@
         <v>8.9720999999999995E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>144</v>
       </c>
@@ -15540,7 +15541,7 @@
         <v>0.111415</v>
       </c>
     </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>144</v>
       </c>
@@ -15623,7 +15624,7 @@
         <v>0.133185</v>
       </c>
     </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>144</v>
       </c>
@@ -15706,7 +15707,7 @@
         <v>0.15523600000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>144</v>
       </c>
@@ -15789,7 +15790,7 @@
         <v>0.17766699999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>144</v>
       </c>
@@ -15872,7 +15873,7 @@
         <v>0.20032700000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>144</v>
       </c>
@@ -15955,7 +15956,7 @@
         <v>0.22278400000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>144</v>
       </c>
@@ -16038,7 +16039,7 @@
         <v>0.245505</v>
       </c>
     </row>
-    <row r="191" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>144</v>
       </c>
@@ -16121,7 +16122,7 @@
         <v>0.26843400000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>157</v>
       </c>
@@ -16129,7 +16130,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="193" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>157</v>
       </c>
@@ -16212,7 +16213,7 @@
         <v>-0.123839</v>
       </c>
     </row>
-    <row r="194" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>157</v>
       </c>
@@ -16295,7 +16296,7 @@
         <v>-0.12081600000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>157</v>
       </c>
@@ -16378,7 +16379,7 @@
         <v>-0.111315</v>
       </c>
     </row>
-    <row r="196" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>157</v>
       </c>
@@ -16461,7 +16462,7 @@
         <v>-9.7583000000000003E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>157</v>
       </c>
@@ -16544,7 +16545,7 @@
         <v>-8.3023E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>157</v>
       </c>
@@ -16627,7 +16628,7 @@
         <v>-6.5462000000000006E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>157</v>
       </c>
@@ -16710,7 +16711,7 @@
         <v>-4.5982000000000002E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>157</v>
       </c>
@@ -16793,7 +16794,7 @@
         <v>-2.5416000000000001E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>157</v>
       </c>
@@ -16876,7 +16877,7 @@
         <v>-5.0930000000000003E-3</v>
       </c>
     </row>
-    <row r="202" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>157</v>
       </c>
@@ -16959,7 +16960,7 @@
         <v>1.5464E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>157</v>
       </c>
@@ -17042,7 +17043,7 @@
         <v>3.4377999999999999E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>157</v>
       </c>
@@ -17125,7 +17126,7 @@
         <v>5.7707000000000001E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>157</v>
       </c>
@@ -17208,7 +17209,7 @@
         <v>7.9015000000000002E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>157</v>
       </c>
@@ -17291,7 +17292,7 @@
         <v>0.10055</v>
       </c>
     </row>
-    <row r="207" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>157</v>
       </c>
@@ -17374,7 +17375,7 @@
         <v>0.122318</v>
       </c>
     </row>
-    <row r="208" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>157</v>
       </c>
@@ -17457,7 +17458,7 @@
         <v>0.14458499999999999</v>
       </c>
     </row>
-    <row r="209" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>157</v>
       </c>
@@ -17540,7 +17541,7 @@
         <v>0.166549</v>
       </c>
     </row>
-    <row r="210" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>157</v>
       </c>
@@ -17623,7 +17624,7 @@
         <v>0.18903400000000001</v>
       </c>
     </row>
-    <row r="211" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>157</v>
       </c>
@@ -17706,7 +17707,7 @@
         <v>0.21138399999999999</v>
       </c>
     </row>
-    <row r="212" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>157</v>
       </c>
@@ -17789,7 +17790,7 @@
         <v>0.233959</v>
       </c>
     </row>
-    <row r="213" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>170</v>
       </c>
@@ -17797,7 +17798,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="214" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>170</v>
       </c>
@@ -17880,7 +17881,7 @@
         <v>-0.117699</v>
       </c>
     </row>
-    <row r="215" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>170</v>
       </c>
@@ -17963,7 +17964,7 @@
         <v>-0.125782</v>
       </c>
     </row>
-    <row r="216" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>170</v>
       </c>
@@ -18046,7 +18047,7 @@
         <v>-0.125503</v>
       </c>
     </row>
-    <row r="217" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>170</v>
       </c>
@@ -18129,7 +18130,7 @@
         <v>-0.11867999999999999</v>
       </c>
     </row>
-    <row r="218" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>170</v>
       </c>
@@ -18212,7 +18213,7 @@
         <v>-0.103688</v>
       </c>
     </row>
-    <row r="219" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>170</v>
       </c>
@@ -18295,7 +18296,7 @@
         <v>-8.9559E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>170</v>
       </c>
@@ -18378,7 +18379,7 @@
         <v>-7.2054999999999994E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>170</v>
       </c>
@@ -18461,7 +18462,7 @@
         <v>-5.3304999999999998E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>170</v>
       </c>
@@ -18544,7 +18545,7 @@
         <v>-3.5407000000000001E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>170</v>
       </c>
@@ -18627,7 +18628,7 @@
         <v>-1.3498E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>170</v>
       </c>
@@ -18710,7 +18711,7 @@
         <v>7.404E-3</v>
       </c>
     </row>
-    <row r="225" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>170</v>
       </c>
@@ -18793,7 +18794,7 @@
         <v>2.7826E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>170</v>
       </c>
@@ -18876,7 +18877,7 @@
         <v>4.8805000000000001E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>170</v>
       </c>
@@ -18959,7 +18960,7 @@
         <v>6.8862999999999994E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>170</v>
       </c>
@@ -19042,7 +19043,7 @@
         <v>9.1355000000000006E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>170</v>
       </c>
@@ -19125,7 +19126,7 @@
         <v>0.11316900000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>170</v>
       </c>
@@ -19208,7 +19209,7 @@
         <v>0.13489399999999999</v>
       </c>
     </row>
-    <row r="231" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>170</v>
       </c>
@@ -19291,7 +19292,7 @@
         <v>0.15700700000000001</v>
       </c>
     </row>
-    <row r="232" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>170</v>
       </c>
@@ -19374,7 +19375,7 @@
         <v>0.17932699999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>170</v>
       </c>
@@ -19457,7 +19458,7 @@
         <v>0.20153199999999999</v>
       </c>
     </row>
-    <row r="234" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>183</v>
       </c>
@@ -19465,7 +19466,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="235" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>183</v>
       </c>
@@ -19548,7 +19549,7 @@
         <v>-0.114605</v>
       </c>
     </row>
-    <row r="236" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>183</v>
       </c>
@@ -19631,7 +19632,7 @@
         <v>-0.123192</v>
       </c>
     </row>
-    <row r="237" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>183</v>
       </c>
@@ -19714,7 +19715,7 @@
         <v>-0.13151299999999999</v>
       </c>
     </row>
-    <row r="238" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>183</v>
       </c>
@@ -19797,7 +19798,7 @@
         <v>-0.129218</v>
       </c>
     </row>
-    <row r="239" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>183</v>
       </c>
@@ -19880,7 +19881,7 @@
         <v>-0.12070699999999999</v>
       </c>
     </row>
-    <row r="240" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>183</v>
       </c>
@@ -19963,7 +19964,7 @@
         <v>-0.108503</v>
       </c>
     </row>
-    <row r="241" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>183</v>
       </c>
@@ -20046,7 +20047,7 @@
         <v>-9.4513E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>183</v>
       </c>
@@ -20129,7 +20130,7 @@
         <v>-7.7424999999999994E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>183</v>
       </c>
@@ -20212,7 +20213,7 @@
         <v>-5.9497000000000001E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>183</v>
       </c>
@@ -20295,7 +20296,7 @@
         <v>-4.1619999999999997E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>183</v>
       </c>
@@ -20378,7 +20379,7 @@
         <v>-2.0154999999999999E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>183</v>
       </c>
@@ -20461,7 +20462,7 @@
         <v>-1.7979999999999999E-3</v>
       </c>
     </row>
-    <row r="247" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>183</v>
       </c>
@@ -20544,7 +20545,7 @@
         <v>2.0473999999999999E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>183</v>
       </c>
@@ -20627,7 +20628,7 @@
         <v>4.0411999999999997E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>183</v>
       </c>
@@ -20710,7 +20711,7 @@
         <v>6.2199999999999998E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>183</v>
       </c>
@@ -20793,7 +20794,7 @@
         <v>8.3400000000000002E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>183</v>
       </c>
@@ -20876,7 +20877,7 @@
         <v>0.105175</v>
       </c>
     </row>
-    <row r="252" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>183</v>
       </c>
@@ -20959,7 +20960,7 @@
         <v>0.126864</v>
       </c>
     </row>
-    <row r="253" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>183</v>
       </c>
@@ -21042,7 +21043,7 @@
         <v>0.14877899999999999</v>
       </c>
     </row>
-    <row r="254" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>183</v>
       </c>
@@ -21125,7 +21126,7 @@
         <v>0.17086999999999999</v>
       </c>
     </row>
-    <row r="255" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
         <v>196</v>
       </c>
@@ -21133,7 +21134,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="256" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>196</v>
       </c>
@@ -21216,7 +21217,7 @@
         <v>-0.107599</v>
       </c>
     </row>
-    <row r="257" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>196</v>
       </c>
@@ -21299,7 +21300,7 @@
         <v>-0.116814</v>
       </c>
     </row>
-    <row r="258" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>196</v>
       </c>
@@ -21382,7 +21383,7 @@
         <v>-0.124041</v>
       </c>
     </row>
-    <row r="259" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>196</v>
       </c>
@@ -21465,7 +21466,7 @@
         <v>-0.13381000000000001</v>
       </c>
     </row>
-    <row r="260" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>196</v>
       </c>
@@ -21548,7 +21549,7 @@
         <v>-0.134129</v>
       </c>
     </row>
-    <row r="261" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>196</v>
       </c>
@@ -21631,7 +21632,7 @@
         <v>-0.12496599999999999</v>
       </c>
     </row>
-    <row r="262" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>196</v>
       </c>
@@ -21714,7 +21715,7 @@
         <v>-0.11374099999999999</v>
       </c>
     </row>
-    <row r="263" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>196</v>
       </c>
@@ -21797,7 +21798,7 @@
         <v>-9.9589999999999998E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>196</v>
       </c>
@@ -21880,7 +21881,7 @@
         <v>-8.2210000000000005E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>196</v>
       </c>
@@ -21963,7 +21964,7 @@
         <v>-6.4680000000000001E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>196</v>
       </c>
@@ -22046,7 +22047,7 @@
         <v>-4.4600000000000001E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>196</v>
       </c>
@@ -22129,7 +22130,7 @@
         <v>-2.7432000000000002E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>196</v>
       </c>
@@ -22212,7 +22213,7 @@
         <v>-5.7549999999999997E-3</v>
       </c>
     </row>
-    <row r="269" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>196</v>
       </c>
@@ -22295,7 +22296,7 @@
         <v>1.4517E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>196</v>
       </c>
@@ -22378,7 +22379,7 @@
         <v>3.5138999999999997E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>196</v>
       </c>
@@ -22461,7 +22462,7 @@
         <v>5.595E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>196</v>
       </c>
@@ -22544,7 +22545,7 @@
         <v>7.7256000000000005E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>196</v>
       </c>
@@ -22627,7 +22628,7 @@
         <v>9.8601999999999995E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>196</v>
       </c>
@@ -22710,7 +22711,7 @@
         <v>0.120076</v>
       </c>
     </row>
-    <row r="275" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>196</v>
       </c>
@@ -22793,7 +22794,7 @@
         <v>0.142039</v>
       </c>
     </row>
-    <row r="276" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2">
         <v>209</v>
       </c>
@@ -22801,7 +22802,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="277" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A277" s="2">
         <v>209</v>
       </c>
@@ -22809,7 +22810,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="278" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>209</v>
       </c>
@@ -22892,7 +22893,7 @@
         <v>-0.112792</v>
       </c>
     </row>
-    <row r="279" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>209</v>
       </c>
@@ -22975,7 +22976,7 @@
         <v>-0.12010999999999999</v>
       </c>
     </row>
-    <row r="280" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>209</v>
       </c>
@@ -23058,7 +23059,7 @@
         <v>-0.128556</v>
       </c>
     </row>
-    <row r="281" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>209</v>
       </c>
@@ -23141,7 +23142,7 @@
         <v>-0.13279099999999999</v>
       </c>
     </row>
-    <row r="282" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>209</v>
       </c>
@@ -23224,7 +23225,7 @@
         <v>-0.133185</v>
       </c>
     </row>
-    <row r="283" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>209</v>
       </c>
@@ -23307,7 +23308,7 @@
         <v>-0.12953600000000001</v>
       </c>
     </row>
-    <row r="284" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>209</v>
       </c>
@@ -23390,7 +23391,7 @@
         <v>-0.116392</v>
       </c>
     </row>
-    <row r="285" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>209</v>
       </c>
@@ -23473,7 +23474,7 @@
         <v>-0.10116</v>
       </c>
     </row>
-    <row r="286" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>209</v>
       </c>
@@ -23556,7 +23557,7 @@
         <v>-8.6471000000000006E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>209</v>
       </c>
@@ -23639,7 +23640,7 @@
         <v>-6.9404999999999994E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>209</v>
       </c>
@@ -23722,7 +23723,7 @@
         <v>-4.9056000000000002E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>209</v>
       </c>
@@ -23805,7 +23806,7 @@
         <v>-3.0010999999999999E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>209</v>
       </c>
@@ -23888,7 +23889,7 @@
         <v>-1.0146000000000001E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>209</v>
       </c>
@@ -23971,7 +23972,7 @@
         <v>9.7429999999999999E-3</v>
       </c>
     </row>
-    <row r="292" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>209</v>
       </c>
@@ -24054,7 +24055,7 @@
         <v>3.0131000000000002E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>209</v>
       </c>
@@ -24137,7 +24138,7 @@
         <v>5.0723999999999998E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>209</v>
       </c>
@@ -24220,7 +24221,7 @@
         <v>7.1836999999999998E-2</v>
       </c>
     </row>
-    <row r="295" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>209</v>
       </c>
@@ -24303,7 +24304,7 @@
         <v>9.3066999999999997E-2</v>
       </c>
     </row>
-    <row r="296" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>209</v>
       </c>
@@ -24386,7 +24387,7 @@
         <v>0.114011</v>
       </c>
     </row>
-    <row r="297" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2">
         <v>222</v>
       </c>
@@ -24394,7 +24395,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="298" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2">
         <v>222</v>
       </c>
@@ -24402,7 +24403,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="299" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>222</v>
       </c>
@@ -24485,7 +24486,7 @@
         <v>-0.108665</v>
       </c>
     </row>
-    <row r="300" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>222</v>
       </c>
@@ -24568,7 +24569,7 @@
         <v>-0.115304</v>
       </c>
     </row>
-    <row r="301" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>222</v>
       </c>
@@ -24651,7 +24652,7 @@
         <v>-0.122076</v>
       </c>
     </row>
-    <row r="302" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>222</v>
       </c>
@@ -24734,7 +24735,7 @@
         <v>-0.13081799999999999</v>
       </c>
     </row>
-    <row r="303" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>222</v>
       </c>
@@ -24817,7 +24818,7 @@
         <v>-0.13634199999999999</v>
       </c>
     </row>
-    <row r="304" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>222</v>
       </c>
@@ -24900,7 +24901,7 @@
         <v>-0.13533899999999999</v>
       </c>
     </row>
-    <row r="305" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>222</v>
       </c>
@@ -24983,7 +24984,7 @@
         <v>-0.12890199999999999</v>
       </c>
     </row>
-    <row r="306" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>222</v>
       </c>
@@ -25066,7 +25067,7 @@
         <v>-0.119807</v>
       </c>
     </row>
-    <row r="307" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>222</v>
       </c>
@@ -25149,7 +25150,7 @@
         <v>-0.10430399999999999</v>
       </c>
     </row>
-    <row r="308" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>222</v>
       </c>
@@ -25232,7 +25233,7 @@
         <v>-8.8673000000000002E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>222</v>
       </c>
@@ -25315,7 +25316,7 @@
         <v>-7.0440000000000003E-2</v>
       </c>
     </row>
-    <row r="310" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>222</v>
       </c>
@@ -25398,7 +25399,7 @@
         <v>-5.2276999999999997E-2</v>
       </c>
     </row>
-    <row r="311" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>222</v>
       </c>
@@ -25481,7 +25482,7 @@
         <v>-3.3048000000000001E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>222</v>
       </c>
@@ -25564,7 +25565,7 @@
         <v>-1.3840999999999999E-2</v>
       </c>
     </row>
-    <row r="313" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>222</v>
       </c>
@@ -25647,7 +25648,7 @@
         <v>6.0270000000000002E-3</v>
       </c>
     </row>
-    <row r="314" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>222</v>
       </c>
@@ -25730,7 +25731,7 @@
         <v>2.6072000000000001E-2</v>
       </c>
     </row>
-    <row r="315" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>222</v>
       </c>
@@ -25813,7 +25814,7 @@
         <v>4.6800000000000001E-2</v>
       </c>
     </row>
-    <row r="316" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>222</v>
       </c>
@@ -25896,7 +25897,7 @@
         <v>6.7734000000000003E-2</v>
       </c>
     </row>
-    <row r="317" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>222</v>
       </c>
@@ -25979,7 +25980,7 @@
         <v>6.7734000000000003E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A318" s="2">
         <v>235</v>
       </c>
@@ -25987,7 +25988,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="319" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A319" s="2">
         <v>235</v>
       </c>
@@ -25995,7 +25996,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="320" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>235</v>
       </c>
@@ -26078,7 +26079,7 @@
         <v>-0.106501</v>
       </c>
     </row>
-    <row r="321" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>235</v>
       </c>
@@ -26161,7 +26162,7 @@
         <v>-0.10943899999999999</v>
       </c>
     </row>
-    <row r="322" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>235</v>
       </c>
@@ -26244,7 +26245,7 @@
         <v>-0.115009</v>
       </c>
     </row>
-    <row r="323" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>235</v>
       </c>
@@ -26327,7 +26328,7 @@
         <v>-0.122445</v>
       </c>
     </row>
-    <row r="324" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>235</v>
       </c>
@@ -26410,7 +26411,7 @@
         <v>-0.131325</v>
       </c>
     </row>
-    <row r="325" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>235</v>
       </c>
@@ -26493,7 +26494,7 @@
         <v>-0.13451099999999999</v>
       </c>
     </row>
-    <row r="326" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>235</v>
       </c>
@@ -26576,7 +26577,7 @@
         <v>-0.13647100000000001</v>
       </c>
     </row>
-    <row r="327" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>235</v>
       </c>
@@ -26659,7 +26660,7 @@
         <v>-0.12968199999999999</v>
       </c>
     </row>
-    <row r="328" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>235</v>
       </c>
@@ -26742,7 +26743,7 @@
         <v>-0.119564</v>
       </c>
     </row>
-    <row r="329" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>235</v>
       </c>
@@ -26825,7 +26826,7 @@
         <v>-0.104155</v>
       </c>
     </row>
-    <row r="330" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>235</v>
       </c>
@@ -26908,7 +26909,7 @@
         <v>-9.0645000000000003E-2</v>
       </c>
     </row>
-    <row r="331" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>235</v>
       </c>
@@ -26991,7 +26992,7 @@
         <v>-7.3552000000000006E-2</v>
       </c>
     </row>
-    <row r="332" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>235</v>
       </c>
@@ -27074,7 +27075,7 @@
         <v>-5.4515000000000001E-2</v>
       </c>
     </row>
-    <row r="333" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>235</v>
       </c>
@@ -27157,7 +27158,7 @@
         <v>-3.5671000000000001E-2</v>
       </c>
     </row>
-    <row r="334" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>235</v>
       </c>
@@ -27240,7 +27241,7 @@
         <v>-1.6115999999999998E-2</v>
       </c>
     </row>
-    <row r="335" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>235</v>
       </c>
@@ -27323,7 +27324,7 @@
         <v>3.2820000000000002E-3</v>
       </c>
     </row>
-    <row r="336" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>235</v>
       </c>
@@ -27406,7 +27407,7 @@
         <v>2.3609999999999999E-2</v>
       </c>
     </row>
-    <row r="337" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>235</v>
       </c>
@@ -27489,7 +27490,7 @@
         <v>4.4012000000000003E-2</v>
       </c>
     </row>
-    <row r="338" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>235</v>
       </c>
@@ -27572,7 +27573,7 @@
         <v>6.4711000000000005E-2</v>
       </c>
     </row>
-    <row r="339" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A339" s="2">
         <v>248</v>
       </c>
@@ -27580,7 +27581,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="340" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A340" s="2">
         <v>248</v>
       </c>
@@ -27588,7 +27589,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="341" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>248</v>
       </c>
@@ -27671,7 +27672,7 @@
         <v>-0.102488</v>
       </c>
     </row>
-    <row r="342" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>248</v>
       </c>
@@ -27754,7 +27755,7 @@
         <v>-0.10473300000000001</v>
       </c>
     </row>
-    <row r="343" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>248</v>
       </c>
@@ -27837,7 +27838,7 @@
         <v>-0.11043699999999999</v>
       </c>
     </row>
-    <row r="344" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>248</v>
       </c>
@@ -27920,7 +27921,7 @@
         <v>-0.116581</v>
       </c>
     </row>
-    <row r="345" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>248</v>
       </c>
@@ -28003,7 +28004,7 @@
         <v>-0.12124699999999999</v>
       </c>
     </row>
-    <row r="346" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>248</v>
       </c>
@@ -28086,7 +28087,7 @@
         <v>-0.132353</v>
       </c>
     </row>
-    <row r="347" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>248</v>
       </c>
@@ -28169,7 +28170,7 @@
         <v>-0.13736699999999999</v>
       </c>
     </row>
-    <row r="348" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>248</v>
       </c>
@@ -28252,7 +28253,7 @@
         <v>-0.13792399999999999</v>
       </c>
     </row>
-    <row r="349" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>248</v>
       </c>
@@ -28335,7 +28336,7 @@
         <v>-0.129409</v>
       </c>
     </row>
-    <row r="350" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>248</v>
       </c>
@@ -28418,7 +28419,7 @@
         <v>-0.119294</v>
       </c>
     </row>
-    <row r="351" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>248</v>
       </c>
@@ -28501,7 +28502,7 @@
         <v>-0.106186</v>
       </c>
     </row>
-    <row r="352" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>248</v>
       </c>
@@ -28584,7 +28585,7 @@
         <v>-9.0529999999999999E-2</v>
       </c>
     </row>
-    <row r="353" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>248</v>
       </c>
@@ -28667,7 +28668,7 @@
         <v>-7.3513999999999996E-2</v>
       </c>
     </row>
-    <row r="354" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>248</v>
       </c>
@@ -28750,7 +28751,7 @@
         <v>-5.5786000000000002E-2</v>
       </c>
     </row>
-    <row r="355" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>248</v>
       </c>
@@ -28833,7 +28834,7 @@
         <v>-3.7094000000000002E-2</v>
       </c>
     </row>
-    <row r="356" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>248</v>
       </c>
@@ -28916,7 +28917,7 @@
         <v>-1.8197000000000001E-2</v>
       </c>
     </row>
-    <row r="357" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>248</v>
       </c>
@@ -28999,7 +29000,7 @@
         <v>1.9E-3</v>
       </c>
     </row>
-    <row r="358" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>248</v>
       </c>
@@ -29082,7 +29083,7 @@
         <v>2.1600999999999999E-2</v>
       </c>
     </row>
-    <row r="359" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>248</v>
       </c>
@@ -29165,7 +29166,7 @@
         <v>4.1821999999999998E-2</v>
       </c>
     </row>
-    <row r="360" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A360" s="2">
         <v>261</v>
       </c>
@@ -29173,7 +29174,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="361" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A361" s="2">
         <v>261</v>
       </c>
@@ -29181,7 +29182,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="362" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A362" s="2">
         <v>261</v>
       </c>
@@ -29189,7 +29190,7 @@
         <v>92000</v>
       </c>
     </row>
-    <row r="363" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>261</v>
       </c>
@@ -29272,7 +29273,7 @@
         <v>-0.100991</v>
       </c>
     </row>
-    <row r="364" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>261</v>
       </c>
@@ -29355,7 +29356,7 @@
         <v>-0.105363</v>
       </c>
     </row>
-    <row r="365" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>261</v>
       </c>
@@ -29438,7 +29439,7 @@
         <v>-0.112384</v>
       </c>
     </row>
-    <row r="366" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>261</v>
       </c>
@@ -29521,7 +29522,7 @@
         <v>-0.117363</v>
       </c>
     </row>
-    <row r="367" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>261</v>
       </c>
@@ -29604,7 +29605,7 @@
         <v>-0.123393</v>
       </c>
     </row>
-    <row r="368" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>261</v>
       </c>
@@ -29687,7 +29688,7 @@
         <v>-0.13516900000000001</v>
       </c>
     </row>
-    <row r="369" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>261</v>
       </c>
@@ -29770,7 +29771,7 @@
         <v>-0.13525799999999999</v>
       </c>
     </row>
-    <row r="370" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>261</v>
       </c>
@@ -29853,7 +29854,7 @@
         <v>-0.13727200000000001</v>
       </c>
     </row>
-    <row r="371" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>261</v>
       </c>
@@ -29936,7 +29937,7 @@
         <v>-0.12842400000000001</v>
       </c>
     </row>
-    <row r="372" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>261</v>
       </c>
@@ -30019,7 +30020,7 @@
         <v>-0.12216399999999999</v>
       </c>
     </row>
-    <row r="373" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>261</v>
       </c>
@@ -30102,7 +30103,7 @@
         <v>-0.107362</v>
       </c>
     </row>
-    <row r="374" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>261</v>
       </c>
@@ -30185,7 +30186,7 @@
         <v>-9.0858999999999995E-2</v>
       </c>
     </row>
-    <row r="375" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>261</v>
       </c>
@@ -30268,7 +30269,7 @@
         <v>-7.3379E-2</v>
       </c>
     </row>
-    <row r="376" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>261</v>
       </c>
@@ -30351,7 +30352,7 @@
         <v>-5.6509999999999998E-2</v>
       </c>
     </row>
-    <row r="377" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>261</v>
       </c>
@@ -30434,7 +30435,7 @@
         <v>-3.7815000000000001E-2</v>
       </c>
     </row>
-    <row r="378" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>261</v>
       </c>
@@ -30517,7 +30518,7 @@
         <v>-1.8679999999999999E-2</v>
       </c>
     </row>
-    <row r="379" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>261</v>
       </c>
@@ -30600,7 +30601,7 @@
         <v>4.6000000000000001E-4</v>
       </c>
     </row>
-    <row r="380" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>261</v>
       </c>
@@ -30683,7 +30684,7 @@
         <v>2.0589E-2</v>
       </c>
     </row>
-    <row r="381" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A381" s="2">
         <v>274</v>
       </c>
@@ -30691,7 +30692,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="382" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A382" s="2">
         <v>274</v>
       </c>
@@ -30699,7 +30700,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="383" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A383" s="2">
         <v>274</v>
       </c>
@@ -30707,7 +30708,7 @@
         <v>92000</v>
       </c>
     </row>
-    <row r="384" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>274</v>
       </c>
@@ -30790,7 +30791,7 @@
         <v>-9.9690000000000001E-2</v>
       </c>
     </row>
-    <row r="385" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>274</v>
       </c>
@@ -30873,7 +30874,7 @@
         <v>-0.10183</v>
       </c>
     </row>
-    <row r="386" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>274</v>
       </c>
@@ -30956,7 +30957,7 @@
         <v>-0.105709</v>
       </c>
     </row>
-    <row r="387" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>274</v>
       </c>
@@ -31039,7 +31040,7 @@
         <v>-0.11104</v>
       </c>
     </row>
-    <row r="388" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>274</v>
       </c>
@@ -31122,7 +31123,7 @@
         <v>-0.11747299999999999</v>
       </c>
     </row>
-    <row r="389" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>274</v>
       </c>
@@ -31205,7 +31206,7 @@
         <v>-0.123289</v>
       </c>
     </row>
-    <row r="390" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>274</v>
       </c>
@@ -31288,7 +31289,7 @@
         <v>-0.131578</v>
       </c>
     </row>
-    <row r="391" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>274</v>
       </c>
@@ -31371,7 +31372,7 @@
         <v>-0.13652800000000001</v>
       </c>
     </row>
-    <row r="392" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>274</v>
       </c>
@@ -31454,7 +31455,7 @@
         <v>-0.13523299999999999</v>
       </c>
     </row>
-    <row r="393" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>274</v>
       </c>
@@ -31537,7 +31538,7 @@
         <v>-0.1278</v>
       </c>
     </row>
-    <row r="394" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>274</v>
       </c>
@@ -31620,7 +31621,7 @@
         <v>-0.11802799999999999</v>
       </c>
     </row>
-    <row r="395" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>274</v>
       </c>
@@ -31703,7 +31704,7 @@
         <v>-0.104197</v>
       </c>
     </row>
-    <row r="396" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>274</v>
       </c>
@@ -31786,7 +31787,7 @@
         <v>-8.9080999999999994E-2</v>
       </c>
     </row>
-    <row r="397" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>274</v>
       </c>
@@ -31869,7 +31870,7 @@
         <v>-7.3340000000000002E-2</v>
       </c>
     </row>
-    <row r="398" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>274</v>
       </c>
@@ -31952,7 +31953,7 @@
         <v>-5.7070999999999997E-2</v>
       </c>
     </row>
-    <row r="399" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>274</v>
       </c>
@@ -32035,7 +32036,7 @@
         <v>-3.7218000000000001E-2</v>
       </c>
     </row>
-    <row r="400" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>274</v>
       </c>
@@ -32118,7 +32119,7 @@
         <v>-1.8564000000000001E-2</v>
       </c>
     </row>
-    <row r="401" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>274</v>
       </c>
@@ -32201,7 +32202,7 @@
         <v>7.0399999999999998E-4</v>
       </c>
     </row>
-    <row r="402" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A402" s="2">
         <v>287</v>
       </c>
@@ -32209,7 +32210,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="403" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A403" s="2">
         <v>287</v>
       </c>
@@ -32217,7 +32218,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="404" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A404" s="2">
         <v>287</v>
       </c>
@@ -32225,7 +32226,7 @@
         <v>92000</v>
       </c>
     </row>
-    <row r="405" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A405" s="3">
         <v>287</v>
       </c>
@@ -32308,7 +32309,7 @@
         <v>-9.7243999999999997E-2</v>
       </c>
     </row>
-    <row r="406" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>287</v>
       </c>
@@ -32391,7 +32392,7 @@
         <v>-9.8048999999999997E-2</v>
       </c>
     </row>
-    <row r="407" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>287</v>
       </c>
@@ -32474,7 +32475,7 @@
         <v>-0.102283</v>
       </c>
     </row>
-    <row r="408" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>287</v>
       </c>
@@ -32557,7 +32558,7 @@
         <v>-0.107113</v>
       </c>
     </row>
-    <row r="409" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>287</v>
       </c>
@@ -32640,7 +32641,7 @@
         <v>-0.11071400000000001</v>
       </c>
     </row>
-    <row r="410" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>287</v>
       </c>
@@ -32723,7 +32724,7 @@
         <v>-0.12119099999999999</v>
       </c>
     </row>
-    <row r="411" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>287</v>
       </c>
@@ -32806,7 +32807,7 @@
         <v>-0.12559200000000001</v>
       </c>
     </row>
-    <row r="412" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>287</v>
       </c>
@@ -32889,7 +32890,7 @@
         <v>-0.128412</v>
       </c>
     </row>
-    <row r="413" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>287</v>
       </c>
@@ -32972,7 +32973,7 @@
         <v>-0.13644000000000001</v>
       </c>
     </row>
-    <row r="414" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>287</v>
       </c>
@@ -33055,7 +33056,7 @@
         <v>-0.13481899999999999</v>
       </c>
     </row>
-    <row r="415" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>287</v>
       </c>
@@ -33138,7 +33139,7 @@
         <v>-0.125142</v>
       </c>
     </row>
-    <row r="416" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>287</v>
       </c>
@@ -33221,7 +33222,7 @@
         <v>-0.115707</v>
       </c>
     </row>
-    <row r="417" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>287</v>
       </c>
@@ -33304,90 +33305,90 @@
         <v>-0.103187</v>
       </c>
     </row>
-    <row r="418" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A418" s="4">
         <v>287</v>
       </c>
       <c r="B418" s="4">
         <v>176000</v>
       </c>
-      <c r="C418" s="4">
+      <c r="C418">
         <v>861</v>
       </c>
-      <c r="D418" s="4">
-        <v>170000</v>
-      </c>
-      <c r="E418" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F418" s="4">
+      <c r="D418">
+        <v>176000</v>
+      </c>
+      <c r="E418">
+        <v>0.1</v>
+      </c>
+      <c r="F418">
         <v>287</v>
       </c>
-      <c r="G418" s="4">
-        <v>4.1812000000000002E-2</v>
-      </c>
-      <c r="H418" s="4">
-        <v>180</v>
-      </c>
-      <c r="I418" s="4">
-        <v>180</v>
-      </c>
-      <c r="J418" s="4">
-        <v>170</v>
-      </c>
-      <c r="K418" s="4">
-        <v>170</v>
-      </c>
-      <c r="L418" s="4">
-        <v>40</v>
-      </c>
-      <c r="M418" s="4">
-        <v>35.001888999999998</v>
-      </c>
-      <c r="N418" s="4">
-        <v>89.263841999999997</v>
-      </c>
-      <c r="O418" s="4">
-        <v>25</v>
-      </c>
-      <c r="P418" s="4">
-        <v>1.8386E-2</v>
-      </c>
-      <c r="Q418" s="4">
-        <v>0.14724200000000001</v>
-      </c>
-      <c r="R418" s="4">
-        <v>0.83437099999999997</v>
-      </c>
-      <c r="S418" s="4">
-        <v>-32151.358345000001</v>
-      </c>
-      <c r="T418" s="4">
-        <v>160213.39095900001</v>
-      </c>
-      <c r="U418" s="4">
-        <v>116237.132598</v>
-      </c>
-      <c r="V418" s="4">
-        <v>34.363059</v>
-      </c>
-      <c r="W418" s="4">
-        <v>50.968797000000002</v>
-      </c>
-      <c r="X418" s="4">
-        <v>17.447009999999999</v>
-      </c>
-      <c r="Y418" s="4">
-        <v>25.118853000000001</v>
-      </c>
-      <c r="Z418" s="4">
-        <v>60.074750000000002</v>
-      </c>
-      <c r="AA418" s="4">
-        <v>-0.103187</v>
-      </c>
-    </row>
-    <row r="419" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="G418" s="5">
+        <v>4.1047701916726999E-2</v>
+      </c>
+      <c r="H418">
+        <v>180</v>
+      </c>
+      <c r="I418">
+        <v>180</v>
+      </c>
+      <c r="J418">
+        <v>170</v>
+      </c>
+      <c r="K418">
+        <v>170</v>
+      </c>
+      <c r="L418">
+        <v>40</v>
+      </c>
+      <c r="M418">
+        <v>35.005543228546202</v>
+      </c>
+      <c r="N418">
+        <v>89.156652456814101</v>
+      </c>
+      <c r="O418">
+        <v>25</v>
+      </c>
+      <c r="P418" s="5">
+        <v>1.7636853289554701E-2</v>
+      </c>
+      <c r="Q418">
+        <v>0.14735447200656701</v>
+      </c>
+      <c r="R418">
+        <v>0.83500867470387796</v>
+      </c>
+      <c r="S418">
+        <v>-36861.7018666882</v>
+      </c>
+      <c r="T418">
+        <v>159281.66924836501</v>
+      </c>
+      <c r="U418">
+        <v>117955.389560435</v>
+      </c>
+      <c r="V418">
+        <v>34.396188132836102</v>
+      </c>
+      <c r="W418">
+        <v>51.016036331708698</v>
+      </c>
+      <c r="X418">
+        <v>17.1138970926567</v>
+      </c>
+      <c r="Y418">
+        <v>25.543966405830201</v>
+      </c>
+      <c r="Z418">
+        <v>62.760723377963103</v>
+      </c>
+      <c r="AA418" s="5">
+        <v>-8.9577405661471501E-2</v>
+      </c>
+    </row>
+    <row r="419" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>287</v>
       </c>
@@ -33470,7 +33471,7 @@
         <v>-7.2483000000000006E-2</v>
       </c>
     </row>
-    <row r="420" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>287</v>
       </c>
@@ -33553,7 +33554,7 @@
         <v>-5.6037999999999998E-2</v>
       </c>
     </row>
-    <row r="421" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>287</v>
       </c>
@@ -33636,7 +33637,7 @@
         <v>-3.6205000000000001E-2</v>
       </c>
     </row>
-    <row r="422" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>287</v>
       </c>
@@ -33719,7 +33720,7 @@
         <v>-1.7988000000000001E-2</v>
       </c>
     </row>
-    <row r="423" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A423" s="2">
         <v>300</v>
       </c>
@@ -33727,7 +33728,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="424" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A424" s="2">
         <v>300</v>
       </c>
@@ -33735,7 +33736,7 @@
         <v>86000</v>
       </c>
     </row>
-    <row r="425" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A425" s="2">
         <v>300</v>
       </c>
@@ -33743,7 +33744,7 @@
         <v>92000</v>
       </c>
     </row>
-    <row r="426" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A426" s="3">
         <v>300</v>
       </c>
@@ -33826,7 +33827,7 @@
         <v>-9.1347999999999999E-2</v>
       </c>
     </row>
-    <row r="427" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>300</v>
       </c>
@@ -33909,7 +33910,7 @@
         <v>-9.5436999999999994E-2</v>
       </c>
     </row>
-    <row r="428" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>300</v>
       </c>
@@ -33992,7 +33993,7 @@
         <v>-9.7256999999999996E-2</v>
       </c>
     </row>
-    <row r="429" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>300</v>
       </c>
@@ -34075,7 +34076,7 @@
         <v>-0.101368</v>
       </c>
     </row>
-    <row r="430" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>300</v>
       </c>
@@ -34158,7 +34159,7 @@
         <v>-0.106861</v>
       </c>
     </row>
-    <row r="431" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>300</v>
       </c>
@@ -34241,7 +34242,7 @@
         <v>-0.11322</v>
       </c>
     </row>
-    <row r="432" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>300</v>
       </c>
@@ -34324,7 +34325,7 @@
         <v>-0.11818099999999999</v>
       </c>
     </row>
-    <row r="433" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>300</v>
       </c>
@@ -34407,7 +34408,7 @@
         <v>-0.124765</v>
       </c>
     </row>
-    <row r="434" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>300</v>
       </c>
@@ -34490,7 +34491,7 @@
         <v>-0.129356</v>
       </c>
     </row>
-    <row r="435" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>300</v>
       </c>
@@ -34573,7 +34574,7 @@
         <v>-0.13395599999999999</v>
       </c>
     </row>
-    <row r="436" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>300</v>
       </c>
@@ -34656,7 +34657,7 @@
         <v>-0.13219400000000001</v>
       </c>
     </row>
-    <row r="437" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>300</v>
       </c>
@@ -34739,7 +34740,7 @@
         <v>-0.12568599999999999</v>
       </c>
     </row>
-    <row r="438" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>300</v>
       </c>
@@ -34822,7 +34823,7 @@
         <v>-0.114414</v>
       </c>
     </row>
-    <row r="439" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>300</v>
       </c>
@@ -34905,7 +34906,7 @@
         <v>-0.10058400000000001</v>
       </c>
     </row>
-    <row r="440" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>300</v>
       </c>
@@ -34988,7 +34989,7 @@
         <v>-8.6503999999999998E-2</v>
       </c>
     </row>
-    <row r="441" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>300</v>
       </c>
@@ -35071,7 +35072,7 @@
         <v>-6.9417999999999994E-2</v>
       </c>
     </row>
-    <row r="442" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>300</v>
       </c>
@@ -35154,7 +35155,7 @@
         <v>-5.3325999999999998E-2</v>
       </c>
     </row>
-    <row r="443" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>300</v>
       </c>
@@ -35244,12 +35245,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>176000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4.1047701916726999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>35.005543228546202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>89.156652456814101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>1.7636853289554701E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.14735447200656701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.83500867470387796</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-36861.7018666882</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>159281.66924836501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>117955.389560435</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>34.396188132836102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>51.016036331708698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17.1138970926567</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>25.543966405830201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>62.760723377963103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>-8.9577405661471501E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -35264,6 +35391,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F19637432BAAAA4E8B613AD4CF549CCD" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1a882fa068e99a90637f35d72ee4199">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f35accf0-cd8f-4670-ac72-d44f2085032d" xmlns:ns4="95507c7c-a837-40bb-8a3d-470d6a1609d2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f9631af341c2920228165fa301a4a4d8" ns3:_="" ns4:_="">
     <xsd:import namespace="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
@@ -35472,12 +35605,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2B5FC1-AD94-452E-B48E-8A2F9B1C8C34}">
   <ds:schemaRefs>
@@ -35487,6 +35614,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A6ED6D0-FE53-4BFC-8DEF-82D0D9F0E993}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="95507c7c-a837-40bb-8a3d-470d6a1609d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0B59684-2680-485A-B9CC-B3EE2FE02703}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35503,21 +35647,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A6ED6D0-FE53-4BFC-8DEF-82D0D9F0E993}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f35accf0-cd8f-4670-ac72-d44f2085032d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="95507c7c-a837-40bb-8a3d-470d6a1609d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>